<commit_message>
Update PDS support file (#1744)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="218">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,733 +145,733 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>电动机及负载标注2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水泵标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>潜水泵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Properties（Include）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFAS810</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lumped Load</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default PF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Roller Shutter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electric Window</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESEW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB114</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC Charger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB131</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC Charger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB006-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB043</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BDB044</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lighting Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emergency Lighting Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electrical Control Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emergency Power Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire Emergency Lighting Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Isolation Switch Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electrical Meter Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL001-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL001-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL045</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL056</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL066</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL042</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL053</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL063</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL302</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL302-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL306</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL306-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL302-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL309</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL309-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL308</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL308-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL305</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL311</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL203-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL204</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL307</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL316</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL315</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL315-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL315-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL312</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL313</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL317-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BL317-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BLITE90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BLITE91</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BLITE91-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BLITE91-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BLITE91-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL102</t>
+  </si>
+  <si>
+    <t>E-BFEL100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL101</t>
+  </si>
+  <si>
+    <t>E-BFEL103</t>
+  </si>
+  <si>
+    <t>E-BFEL110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL111</t>
+  </si>
+  <si>
+    <t>E-BFEL120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL121</t>
+  </si>
+  <si>
+    <t>E-BFEL122</t>
+  </si>
+  <si>
+    <t>E-BFEL123</t>
+  </si>
+  <si>
+    <t>E-BFEL130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL131</t>
+  </si>
+  <si>
+    <t>E-BFEL140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL141</t>
+  </si>
+  <si>
+    <t>E-BFEL161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL161-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL201</t>
+  </si>
+  <si>
+    <t>E-BFEL201-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL211</t>
+  </si>
+  <si>
+    <t>E-BFEL211-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL240</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL241</t>
+  </si>
+  <si>
+    <t>E-BFEL250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL251</t>
+  </si>
+  <si>
+    <t>E-BFEL500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL710</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL800-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL810</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL810-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL811</t>
+  </si>
+  <si>
+    <t>E-BFEL811-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL820</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL820-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL830</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFEL830-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS211</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS211-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS211-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS211-3</t>
+  </si>
+  <si>
+    <t>E-BS301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS311</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS311-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS311-2</t>
+  </si>
+  <si>
+    <t>E-BS311-3</t>
+  </si>
+  <si>
+    <t>E-BS203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS201-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS201-2</t>
+  </si>
+  <si>
+    <t>E-BS204-S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS204</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS205</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS202-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS202-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS209</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS206</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS207</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS302</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS212-S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS312</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS202-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS701</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BS802</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Socket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LV Socket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>电动机及负载标注</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>电动机及负载标注2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>水泵标注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>潜水泵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Properties（Include）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fans</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFAS810</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lumped Load</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Default PF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Roller Shutter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Electric Window</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESEW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB114</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC Charger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB131</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DC Charger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB006-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB015</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB043</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BDB044</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lighting Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>APE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FEL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emergency Lighting Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Electrical Control Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emergency Power Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fire Emergency Lighting Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Isolation Switch Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Electrical Meter Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL001-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL001-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL023</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL015</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL045</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL056</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL066</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL042</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL053</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL063</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL302</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL302-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL306</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL306-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL302-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL309</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL309-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL308</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL308-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL305</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL311</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL203</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL203-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL204</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL307</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL316</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL315</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL315-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL315-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL312</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL313</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL317-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BL317-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BLITE90</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BLITE91</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BLITE91-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BLITE91-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BLITE91-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL102</t>
-  </si>
-  <si>
-    <t>E-BFEL100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL101</t>
-  </si>
-  <si>
-    <t>E-BFEL103</t>
-  </si>
-  <si>
-    <t>E-BFEL110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL111</t>
-  </si>
-  <si>
-    <t>E-BFEL120</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL121</t>
-  </si>
-  <si>
-    <t>E-BFEL122</t>
-  </si>
-  <si>
-    <t>E-BFEL123</t>
-  </si>
-  <si>
-    <t>E-BFEL130</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL131</t>
-  </si>
-  <si>
-    <t>E-BFEL140</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL141</t>
-  </si>
-  <si>
-    <t>E-BFEL161</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL161-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL201</t>
-  </si>
-  <si>
-    <t>E-BFEL201-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL210</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL211</t>
-  </si>
-  <si>
-    <t>E-BFEL211-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL240</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL241</t>
-  </si>
-  <si>
-    <t>E-BFEL250</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL251</t>
-  </si>
-  <si>
-    <t>E-BFEL500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL700</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL710</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL800</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL800-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL810</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL810-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL811</t>
-  </si>
-  <si>
-    <t>E-BFEL811-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL820</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL820-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL830</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BFEL830-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS211</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS211-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS211-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS211-3</t>
-  </si>
-  <si>
-    <t>E-BS301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS311</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS311-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS311-2</t>
-  </si>
-  <si>
-    <t>E-BS311-3</t>
-  </si>
-  <si>
-    <t>E-BS203</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS200</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS201-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS201-2</t>
-  </si>
-  <si>
-    <t>E-BS204-S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS204</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS205</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS202-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS202-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS209</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS206</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS207</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS302</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS212-S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS312</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS202-4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS701</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-BS802</t>
+    <t>Cat.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cat.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luminaire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luminaire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire Emergency Luminaire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire Emergency Luminaire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emergency Luminaire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luminaire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Waterproof Lights</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lane Lights</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outdoor Lights</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要特殊处理（线槽灯）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Residential Distribution Panel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不读属性直接认为是住户配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>负载标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>负载标注2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-电力平面-负荷明细</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Socket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LV Socket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Motor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>电动机及负载标注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cat.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cat.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Luminaire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Luminaire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fire Emergency Luminaire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fire Emergency Luminaire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emergency Luminaire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Luminaire</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Waterproof Lights</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lane Lights</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outdoor Lights</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要特殊处理（线槽灯）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Residential Distribution Panel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>不读属性直接认为是住户配电箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remark</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>负载标注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>负载标注2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1201,9 +1201,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1211,7 +1213,7 @@
     <col min="2" max="2" width="25.625" customWidth="1"/>
     <col min="3" max="3" width="38.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.625" customWidth="1"/>
-    <col min="5" max="5" width="14.875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="5.875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
   </cols>
@@ -1221,52 +1223,67 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>209</v>
       </c>
       <c r="E2" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
       </c>
       <c r="E3" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
       </c>
       <c r="E4" s="1">
         <v>0.8</v>
@@ -1274,27 +1291,33 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="E5" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
       </c>
       <c r="E6" s="1">
         <v>0.8</v>
@@ -1302,27 +1325,33 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
       </c>
       <c r="E7" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
       </c>
       <c r="E8" s="1">
         <v>0.8</v>
@@ -1330,66 +1359,78 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>214</v>
       </c>
       <c r="E9" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>215</v>
       </c>
       <c r="E10" s="1">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
       </c>
       <c r="E11" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
+        <v>195</v>
       </c>
       <c r="E13" s="1">
         <v>0.8</v>
@@ -1397,89 +1438,71 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
       </c>
       <c r="E16" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E17" s="1">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="E18" s="1">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
+        <v>216</v>
       </c>
       <c r="E19" s="1">
         <v>0.8</v>
@@ -1487,33 +1510,21 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>212</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>213</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="E21" s="1">
         <v>0.8</v>
@@ -1521,33 +1532,33 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="E22" s="1">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="E23" s="1">
         <v>0.8</v>
@@ -1555,50 +1566,41 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" t="s">
-        <v>216</v>
+        <v>45</v>
       </c>
       <c r="E24" s="1">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>217</v>
+        <v>45</v>
       </c>
       <c r="E25" s="1">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E26" s="1">
         <v>0.9</v>
@@ -1606,16 +1608,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="E27" s="1">
         <v>0.9</v>
@@ -1623,55 +1622,49 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="E28" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="F28" t="s">
-        <v>212</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="B30" t="s">
-        <v>206</v>
-      </c>
-      <c r="C30" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E30" s="1">
         <v>0.9</v>
-      </c>
-      <c r="F30" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E31" s="1">
         <v>0.9</v>
@@ -1679,10 +1672,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
       </c>
       <c r="E32" s="1">
         <v>0.9</v>
@@ -1690,13 +1686,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E33" s="1">
         <v>0.9</v>
@@ -1707,10 +1703,7 @@
         <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>201</v>
-      </c>
-      <c r="C34" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E34" s="1">
         <v>0.9</v>
@@ -1718,10 +1711,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E35" s="1">
         <v>0.9</v>
@@ -1729,10 +1722,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="C36" t="s">
+        <v>205</v>
       </c>
       <c r="E36" s="1">
         <v>0.9</v>
@@ -1740,13 +1736,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
-      </c>
-      <c r="C37" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E37" s="1">
         <v>0.9</v>
@@ -1754,10 +1747,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E38" s="1">
         <v>0.9</v>
@@ -1765,10 +1758,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E39" s="1">
         <v>0.9</v>
@@ -1776,10 +1769,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E40" s="1">
         <v>0.9</v>
@@ -1787,10 +1780,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E41" s="1">
         <v>0.9</v>
@@ -1798,10 +1791,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E42" s="1">
         <v>0.9</v>
@@ -1809,10 +1802,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E43" s="1">
         <v>0.9</v>
@@ -1820,10 +1813,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E44" s="1">
         <v>0.9</v>
@@ -1831,10 +1824,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E45" s="1">
         <v>0.9</v>
@@ -1842,10 +1835,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E46" s="1">
         <v>0.9</v>
@@ -1853,10 +1846,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E47" s="1">
         <v>0.9</v>
@@ -1864,10 +1857,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E48" s="1">
         <v>0.9</v>
@@ -1875,10 +1868,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E49" s="1">
         <v>0.9</v>
@@ -1886,10 +1879,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E50" s="1">
         <v>0.9</v>
@@ -1897,10 +1890,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="D51" t="s">
+        <v>93</v>
       </c>
       <c r="E51" s="1">
         <v>0.9</v>
@@ -1908,13 +1904,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>201</v>
-      </c>
-      <c r="D52" t="s">
-        <v>95</v>
+        <v>199</v>
+      </c>
+      <c r="C52" t="s">
+        <v>205</v>
       </c>
       <c r="E52" s="1">
         <v>0.9</v>
@@ -1922,13 +1918,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>201</v>
-      </c>
-      <c r="C53" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E53" s="1">
         <v>0.9</v>
@@ -1936,10 +1929,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="C54" t="s">
+        <v>207</v>
       </c>
       <c r="E54" s="1">
         <v>0.9</v>
@@ -1947,13 +1943,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>201</v>
-      </c>
-      <c r="C55" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E55" s="1">
         <v>0.9</v>
@@ -1961,10 +1954,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E56" s="1">
         <v>0.9</v>
@@ -1972,10 +1965,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E57" s="1">
         <v>0.9</v>
@@ -1983,10 +1976,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B58" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E58" s="1">
         <v>0.9</v>
@@ -1994,10 +1987,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B59" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E59" s="1">
         <v>0.9</v>
@@ -2005,10 +1998,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="C60" t="s">
+        <v>205</v>
       </c>
       <c r="E60" s="1">
         <v>0.9</v>
@@ -2016,13 +2012,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B61" t="s">
-        <v>201</v>
-      </c>
-      <c r="C61" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E61" s="1">
         <v>0.9</v>
@@ -2030,10 +2023,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E62" s="1">
         <v>0.9</v>
@@ -2041,10 +2034,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E63" s="1">
         <v>0.9</v>
@@ -2052,10 +2045,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E64" s="1">
         <v>0.9</v>
@@ -2063,10 +2056,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E65" s="1">
         <v>0.9</v>
@@ -2074,10 +2067,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
       </c>
       <c r="E66" s="1">
         <v>0.9</v>
@@ -2085,13 +2081,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
-      </c>
-      <c r="C67" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E67" s="1">
         <v>0.9</v>
@@ -2099,10 +2092,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E68" s="1">
         <v>0.9</v>
@@ -2110,10 +2103,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="D69" t="s">
+        <v>119</v>
       </c>
       <c r="E69" s="1">
         <v>0.9</v>
@@ -2121,13 +2117,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D70" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E70" s="1">
         <v>0.9</v>
@@ -2135,13 +2131,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="C71" t="s">
+        <v>205</v>
       </c>
       <c r="D71" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E71" s="1">
         <v>0.9</v>
@@ -2149,16 +2148,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>118</v>
+      </c>
+      <c r="B72" t="s">
+        <v>199</v>
+      </c>
+      <c r="D72" t="s">
         <v>119</v>
-      </c>
-      <c r="B72" t="s">
-        <v>201</v>
-      </c>
-      <c r="C72" t="s">
-        <v>207</v>
-      </c>
-      <c r="D72" t="s">
-        <v>121</v>
       </c>
       <c r="E72" s="1">
         <v>0.9</v>
@@ -2169,10 +2165,13 @@
         <v>120</v>
       </c>
       <c r="B73" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="C73" t="s">
+        <v>205</v>
       </c>
       <c r="D73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E73" s="1">
         <v>0.9</v>
@@ -2183,13 +2182,10 @@
         <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C74" t="s">
-        <v>207</v>
-      </c>
-      <c r="D74" t="s">
-        <v>121</v>
+        <v>201</v>
       </c>
       <c r="E74" s="1">
         <v>0.9</v>
@@ -2197,10 +2193,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B75" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C75" t="s">
+        <v>201</v>
       </c>
       <c r="E75" s="1">
         <v>0.9</v>
@@ -2208,10 +2207,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B76" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C76" t="s">
+        <v>201</v>
       </c>
       <c r="E76" s="1">
         <v>0.9</v>
@@ -2219,10 +2221,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B77" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C77" t="s">
+        <v>201</v>
       </c>
       <c r="E77" s="1">
         <v>0.9</v>
@@ -2230,10 +2235,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C78" t="s">
+        <v>201</v>
       </c>
       <c r="E78" s="1">
         <v>0.9</v>
@@ -2241,10 +2249,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C79" t="s">
+        <v>201</v>
       </c>
       <c r="E79" s="1">
         <v>0.9</v>
@@ -2252,10 +2263,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C80" t="s">
+        <v>201</v>
       </c>
       <c r="E80" s="1">
         <v>0.9</v>
@@ -2263,10 +2277,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C81" t="s">
+        <v>201</v>
       </c>
       <c r="E81" s="1">
         <v>0.9</v>
@@ -2274,10 +2291,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B82" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C82" t="s">
+        <v>201</v>
       </c>
       <c r="E82" s="1">
         <v>0.9</v>
@@ -2285,10 +2305,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C83" t="s">
+        <v>201</v>
       </c>
       <c r="E83" s="1">
         <v>0.9</v>
@@ -2296,10 +2319,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B84" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C84" t="s">
+        <v>201</v>
       </c>
       <c r="E84" s="1">
         <v>0.9</v>
@@ -2307,10 +2333,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B85" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C85" t="s">
+        <v>201</v>
       </c>
       <c r="E85" s="1">
         <v>0.9</v>
@@ -2318,10 +2347,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B86" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C86" t="s">
+        <v>201</v>
       </c>
       <c r="E86" s="1">
         <v>0.9</v>
@@ -2329,10 +2361,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B87" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C87" t="s">
+        <v>201</v>
       </c>
       <c r="E87" s="1">
         <v>0.9</v>
@@ -2340,10 +2375,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C88" t="s">
+        <v>201</v>
       </c>
       <c r="E88" s="1">
         <v>0.9</v>
@@ -2351,10 +2389,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B89" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C89" t="s">
+        <v>201</v>
       </c>
       <c r="E89" s="1">
         <v>0.9</v>
@@ -2362,10 +2403,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B90" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C90" t="s">
+        <v>201</v>
       </c>
       <c r="E90" s="1">
         <v>0.9</v>
@@ -2373,10 +2417,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B91" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C91" t="s">
+        <v>201</v>
       </c>
       <c r="E91" s="1">
         <v>0.9</v>
@@ -2384,10 +2431,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B92" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C92" t="s">
+        <v>201</v>
       </c>
       <c r="E92" s="1">
         <v>0.9</v>
@@ -2395,10 +2445,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B93" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C93" t="s">
+        <v>201</v>
       </c>
       <c r="E93" s="1">
         <v>0.9</v>
@@ -2406,10 +2459,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C94" t="s">
+        <v>201</v>
       </c>
       <c r="E94" s="1">
         <v>0.9</v>
@@ -2417,10 +2473,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C95" t="s">
+        <v>201</v>
       </c>
       <c r="E95" s="1">
         <v>0.9</v>
@@ -2428,10 +2487,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B96" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C96" t="s">
+        <v>201</v>
       </c>
       <c r="E96" s="1">
         <v>0.9</v>
@@ -2439,10 +2501,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B97" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C97" t="s">
+        <v>201</v>
       </c>
       <c r="E97" s="1">
         <v>0.9</v>
@@ -2450,10 +2515,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B98" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C98" t="s">
+        <v>201</v>
       </c>
       <c r="E98" s="1">
         <v>0.9</v>
@@ -2461,10 +2529,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B99" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C99" t="s">
+        <v>201</v>
       </c>
       <c r="E99" s="1">
         <v>0.9</v>
@@ -2472,10 +2543,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B100" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C100" t="s">
+        <v>201</v>
       </c>
       <c r="E100" s="1">
         <v>0.9</v>
@@ -2483,10 +2557,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B101" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C101" t="s">
+        <v>201</v>
       </c>
       <c r="E101" s="1">
         <v>0.9</v>
@@ -2494,10 +2571,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C102" t="s">
+        <v>201</v>
       </c>
       <c r="E102" s="1">
         <v>0.9</v>
@@ -2505,10 +2585,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B103" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C103" t="s">
+        <v>201</v>
       </c>
       <c r="E103" s="1">
         <v>0.9</v>
@@ -2516,10 +2599,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B104" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C104" t="s">
+        <v>201</v>
+      </c>
+      <c r="D104" t="s">
+        <v>161</v>
       </c>
       <c r="E104" s="1">
         <v>0.9</v>
@@ -2527,13 +2616,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B105" t="s">
-        <v>203</v>
-      </c>
-      <c r="D105" t="s">
-        <v>163</v>
+        <v>199</v>
+      </c>
+      <c r="C105" t="s">
+        <v>201</v>
       </c>
       <c r="E105" s="1">
         <v>0.9</v>
@@ -2541,10 +2630,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C106" t="s">
+        <v>201</v>
+      </c>
+      <c r="D106" t="s">
+        <v>161</v>
       </c>
       <c r="E106" s="1">
         <v>0.9</v>
@@ -2552,13 +2647,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B107" t="s">
-        <v>203</v>
-      </c>
-      <c r="D107" t="s">
-        <v>163</v>
+        <v>199</v>
+      </c>
+      <c r="C107" t="s">
+        <v>201</v>
       </c>
       <c r="E107" s="1">
         <v>0.9</v>
@@ -2566,10 +2661,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B108" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C108" t="s">
+        <v>202</v>
+      </c>
+      <c r="D108" t="s">
+        <v>161</v>
       </c>
       <c r="E108" s="1">
         <v>0.9</v>
@@ -2577,13 +2678,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B109" t="s">
-        <v>204</v>
+        <v>199</v>
+      </c>
+      <c r="C109" t="s">
+        <v>203</v>
       </c>
       <c r="D109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E109" s="1">
         <v>0.9</v>
@@ -2591,13 +2695,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B110" t="s">
-        <v>205</v>
+        <v>199</v>
+      </c>
+      <c r="C110" t="s">
+        <v>202</v>
       </c>
       <c r="D110" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E110" s="1">
         <v>0.9</v>
@@ -2605,13 +2712,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B111" t="s">
-        <v>204</v>
+        <v>199</v>
+      </c>
+      <c r="C111" t="s">
+        <v>202</v>
       </c>
       <c r="D111" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E111" s="1">
         <v>0.9</v>
@@ -2619,13 +2729,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>159</v>
+      </c>
+      <c r="B112" t="s">
+        <v>199</v>
+      </c>
+      <c r="C112" t="s">
+        <v>202</v>
+      </c>
+      <c r="D112" t="s">
         <v>160</v>
-      </c>
-      <c r="B112" t="s">
-        <v>204</v>
-      </c>
-      <c r="D112" t="s">
-        <v>162</v>
       </c>
       <c r="E112" s="1">
         <v>0.9</v>
@@ -2633,24 +2746,21 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>204</v>
-      </c>
-      <c r="D113" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="E113" s="1">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B114" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E114" s="1">
         <v>0.85</v>
@@ -2658,10 +2768,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B115" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E115" s="1">
         <v>0.85</v>
@@ -2669,10 +2779,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B116" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E116" s="1">
         <v>0.85</v>
@@ -2680,10 +2790,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B117" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E117" s="1">
         <v>0.85</v>
@@ -2691,10 +2801,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B118" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E118" s="1">
         <v>0.85</v>
@@ -2702,10 +2812,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B119" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E119" s="1">
         <v>0.85</v>
@@ -2713,10 +2823,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B120" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E120" s="1">
         <v>0.85</v>
@@ -2724,10 +2834,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="B121" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="E121" s="1">
         <v>0.85</v>
@@ -2735,10 +2845,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B122" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E122" s="1">
         <v>0.85</v>
@@ -2746,10 +2856,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B123" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E123" s="1">
         <v>0.85</v>
@@ -2760,7 +2870,7 @@
         <v>179</v>
       </c>
       <c r="B124" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E124" s="1">
         <v>0.85</v>
@@ -2768,10 +2878,10 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B125" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E125" s="1">
         <v>0.85</v>
@@ -2779,10 +2889,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B126" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E126" s="1">
         <v>0.85</v>
@@ -2790,10 +2900,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B127" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E127" s="1">
         <v>0.85</v>
@@ -2801,10 +2911,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E128" s="1">
         <v>0.85</v>
@@ -2812,10 +2922,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B129" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E129" s="1">
         <v>0.85</v>
@@ -2823,10 +2933,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B130" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E130" s="1">
         <v>0.85</v>
@@ -2834,10 +2944,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E131" s="1">
         <v>0.85</v>
@@ -2845,10 +2955,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="B132" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E132" s="1">
         <v>0.85</v>
@@ -2856,10 +2966,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B133" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E133" s="1">
         <v>0.85</v>
@@ -2867,10 +2977,10 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="B134" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E134" s="1">
         <v>0.85</v>
@@ -2878,10 +2988,10 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="B135" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E135" s="1">
         <v>0.85</v>
@@ -2889,10 +2999,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B136" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E136" s="1">
         <v>0.85</v>
@@ -2900,10 +3010,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B137" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E137" s="1">
         <v>0.85</v>
@@ -2911,10 +3021,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B138" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E138" s="1">
         <v>0.85</v>
@@ -2922,10 +3032,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B139" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E139" s="1">
         <v>0.85</v>
@@ -2933,10 +3043,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B140" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E140" s="1">
         <v>0.85</v>
@@ -2947,7 +3057,10 @@
         <v>191</v>
       </c>
       <c r="B141" t="s">
-        <v>195</v>
+        <v>193</v>
+      </c>
+      <c r="C141" t="s">
+        <v>194</v>
       </c>
       <c r="E141" s="1">
         <v>0.85</v>
@@ -2955,26 +3068,12 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>192</v>
+      </c>
+      <c r="B142" t="s">
         <v>193</v>
       </c>
-      <c r="B142" t="s">
-        <v>195</v>
-      </c>
-      <c r="C142" t="s">
-        <v>196</v>
-      </c>
       <c r="E142" s="1">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>194</v>
-      </c>
-      <c r="B143" t="s">
-        <v>195</v>
-      </c>
-      <c r="E143" s="1">
         <v>0.85</v>
       </c>
     </row>
@@ -2990,7 +3089,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B28"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
A  little change (#1750)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="217">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,10 +150,6 @@
   </si>
   <si>
     <t>水泵标注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>潜水泵</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1203,9 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1223,50 +1217,50 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
         <v>197</v>
       </c>
-      <c r="C1" t="s">
-        <v>198</v>
-      </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="F2" t="s">
         <v>209</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>59</v>
       </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1">
         <v>0.85</v>
@@ -1274,16 +1268,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1">
         <v>0.8</v>
@@ -1291,16 +1285,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1">
         <v>0.85</v>
@@ -1308,16 +1302,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1">
         <v>0.8</v>
@@ -1325,16 +1319,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="1">
         <v>0.85</v>
@@ -1342,16 +1336,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1">
         <v>0.8</v>
@@ -1359,16 +1353,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E9" s="1">
         <v>0.85</v>
@@ -1376,16 +1370,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="1">
         <v>0.85</v>
@@ -1393,16 +1387,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="1">
         <v>0.9</v>
@@ -1410,16 +1404,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1">
         <v>0.9</v>
@@ -1430,7 +1424,7 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E13" s="1">
         <v>0.8</v>
@@ -1471,16 +1465,13 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
       <c r="E16" s="1">
         <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -1502,7 +1493,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E19" s="1">
         <v>0.8</v>
@@ -1510,10 +1501,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="1">
         <v>0.8</v>
@@ -1521,10 +1512,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1">
         <v>0.8</v>
@@ -1532,16 +1523,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
       </c>
       <c r="E22" s="1">
         <v>0.8</v>
@@ -1549,16 +1540,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
       <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
         <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
       </c>
       <c r="E23" s="1">
         <v>0.8</v>
@@ -1566,13 +1557,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="1">
         <v>0.9</v>
@@ -1580,13 +1571,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1">
         <v>0.9</v>
@@ -1594,13 +1585,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
         <v>44</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
       </c>
       <c r="E26" s="1">
         <v>0.9</v>
@@ -1608,13 +1599,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
         <v>46</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
       </c>
       <c r="E27" s="1">
         <v>0.9</v>
@@ -1622,10 +1613,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E28" s="1">
         <v>0.9</v>
@@ -1633,27 +1624,27 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E29" s="1">
         <v>0.9</v>
       </c>
       <c r="F29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E30" s="1">
         <v>0.9</v>
@@ -1661,10 +1652,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E31" s="1">
         <v>0.9</v>
@@ -1672,13 +1663,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E32" s="1">
         <v>0.9</v>
@@ -1686,13 +1677,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E33" s="1">
         <v>0.9</v>
@@ -1700,10 +1691,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E34" s="1">
         <v>0.9</v>
@@ -1711,10 +1702,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E35" s="1">
         <v>0.9</v>
@@ -1722,13 +1713,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E36" s="1">
         <v>0.9</v>
@@ -1736,10 +1727,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E37" s="1">
         <v>0.9</v>
@@ -1747,10 +1738,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E38" s="1">
         <v>0.9</v>
@@ -1758,10 +1749,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E39" s="1">
         <v>0.9</v>
@@ -1769,10 +1760,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E40" s="1">
         <v>0.9</v>
@@ -1780,10 +1771,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E41" s="1">
         <v>0.9</v>
@@ -1791,10 +1782,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E42" s="1">
         <v>0.9</v>
@@ -1802,10 +1793,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E43" s="1">
         <v>0.9</v>
@@ -1813,10 +1804,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E44" s="1">
         <v>0.9</v>
@@ -1824,10 +1815,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E45" s="1">
         <v>0.9</v>
@@ -1835,10 +1826,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E46" s="1">
         <v>0.9</v>
@@ -1846,10 +1837,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E47" s="1">
         <v>0.9</v>
@@ -1857,10 +1848,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E48" s="1">
         <v>0.9</v>
@@ -1868,10 +1859,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E49" s="1">
         <v>0.9</v>
@@ -1879,10 +1870,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E50" s="1">
         <v>0.9</v>
@@ -1890,13 +1881,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" t="s">
+        <v>198</v>
+      </c>
+      <c r="D51" t="s">
         <v>92</v>
-      </c>
-      <c r="B51" t="s">
-        <v>199</v>
-      </c>
-      <c r="D51" t="s">
-        <v>93</v>
       </c>
       <c r="E51" s="1">
         <v>0.9</v>
@@ -1904,13 +1895,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E52" s="1">
         <v>0.9</v>
@@ -1918,10 +1909,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E53" s="1">
         <v>0.9</v>
@@ -1929,13 +1920,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E54" s="1">
         <v>0.9</v>
@@ -1943,10 +1934,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E55" s="1">
         <v>0.9</v>
@@ -1954,10 +1945,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E56" s="1">
         <v>0.9</v>
@@ -1965,10 +1956,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E57" s="1">
         <v>0.9</v>
@@ -1976,10 +1967,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E58" s="1">
         <v>0.9</v>
@@ -1987,10 +1978,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E59" s="1">
         <v>0.9</v>
@@ -1998,13 +1989,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E60" s="1">
         <v>0.9</v>
@@ -2012,10 +2003,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E61" s="1">
         <v>0.9</v>
@@ -2023,10 +2014,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E62" s="1">
         <v>0.9</v>
@@ -2034,10 +2025,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E63" s="1">
         <v>0.9</v>
@@ -2045,10 +2036,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E64" s="1">
         <v>0.9</v>
@@ -2056,10 +2047,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E65" s="1">
         <v>0.9</v>
@@ -2067,13 +2058,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E66" s="1">
         <v>0.9</v>
@@ -2081,10 +2072,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E67" s="1">
         <v>0.9</v>
@@ -2092,10 +2083,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E68" s="1">
         <v>0.9</v>
@@ -2103,13 +2094,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E69" s="1">
         <v>0.9</v>
@@ -2117,13 +2108,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E70" s="1">
         <v>0.9</v>
@@ -2131,16 +2122,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E71" s="1">
         <v>0.9</v>
@@ -2148,13 +2139,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" t="s">
+        <v>198</v>
+      </c>
+      <c r="D72" t="s">
         <v>118</v>
-      </c>
-      <c r="B72" t="s">
-        <v>199</v>
-      </c>
-      <c r="D72" t="s">
-        <v>119</v>
       </c>
       <c r="E72" s="1">
         <v>0.9</v>
@@ -2162,16 +2153,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E73" s="1">
         <v>0.9</v>
@@ -2179,13 +2170,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E74" s="1">
         <v>0.9</v>
@@ -2193,13 +2184,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E75" s="1">
         <v>0.9</v>
@@ -2207,13 +2198,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E76" s="1">
         <v>0.9</v>
@@ -2221,13 +2212,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E77" s="1">
         <v>0.9</v>
@@ -2235,13 +2226,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E78" s="1">
         <v>0.9</v>
@@ -2249,13 +2240,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E79" s="1">
         <v>0.9</v>
@@ -2263,13 +2254,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E80" s="1">
         <v>0.9</v>
@@ -2277,13 +2268,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E81" s="1">
         <v>0.9</v>
@@ -2291,13 +2282,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B82" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E82" s="1">
         <v>0.9</v>
@@ -2305,13 +2296,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E83" s="1">
         <v>0.9</v>
@@ -2319,13 +2310,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E84" s="1">
         <v>0.9</v>
@@ -2333,13 +2324,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E85" s="1">
         <v>0.9</v>
@@ -2347,13 +2338,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E86" s="1">
         <v>0.9</v>
@@ -2361,13 +2352,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B87" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E87" s="1">
         <v>0.9</v>
@@ -2375,13 +2366,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E88" s="1">
         <v>0.9</v>
@@ -2389,13 +2380,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E89" s="1">
         <v>0.9</v>
@@ -2403,13 +2394,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E90" s="1">
         <v>0.9</v>
@@ -2417,13 +2408,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E91" s="1">
         <v>0.9</v>
@@ -2431,13 +2422,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E92" s="1">
         <v>0.9</v>
@@ -2445,13 +2436,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B93" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C93" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E93" s="1">
         <v>0.9</v>
@@ -2459,13 +2450,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B94" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E94" s="1">
         <v>0.9</v>
@@ -2473,13 +2464,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E95" s="1">
         <v>0.9</v>
@@ -2487,13 +2478,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E96" s="1">
         <v>0.9</v>
@@ -2501,13 +2492,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B97" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E97" s="1">
         <v>0.9</v>
@@ -2515,13 +2506,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B98" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C98" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E98" s="1">
         <v>0.9</v>
@@ -2529,13 +2520,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E99" s="1">
         <v>0.9</v>
@@ -2543,13 +2534,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B100" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E100" s="1">
         <v>0.9</v>
@@ -2557,13 +2548,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B101" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E101" s="1">
         <v>0.9</v>
@@ -2571,13 +2562,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B102" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E102" s="1">
         <v>0.9</v>
@@ -2585,13 +2576,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B103" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E103" s="1">
         <v>0.9</v>
@@ -2599,16 +2590,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D104" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E104" s="1">
         <v>0.9</v>
@@ -2616,13 +2607,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E105" s="1">
         <v>0.9</v>
@@ -2630,16 +2621,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D106" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E106" s="1">
         <v>0.9</v>
@@ -2647,13 +2638,13 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E107" s="1">
         <v>0.9</v>
@@ -2661,16 +2652,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B108" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D108" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E108" s="1">
         <v>0.9</v>
@@ -2678,16 +2669,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B109" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D109" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E109" s="1">
         <v>0.9</v>
@@ -2695,16 +2686,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B110" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D110" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E110" s="1">
         <v>0.9</v>
@@ -2712,16 +2703,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B111" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C111" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D111" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E111" s="1">
         <v>0.9</v>
@@ -2729,16 +2720,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>158</v>
+      </c>
+      <c r="B112" t="s">
+        <v>198</v>
+      </c>
+      <c r="C112" t="s">
+        <v>201</v>
+      </c>
+      <c r="D112" t="s">
         <v>159</v>
-      </c>
-      <c r="B112" t="s">
-        <v>199</v>
-      </c>
-      <c r="C112" t="s">
-        <v>202</v>
-      </c>
-      <c r="D112" t="s">
-        <v>160</v>
       </c>
       <c r="E112" s="1">
         <v>0.9</v>
@@ -2746,10 +2737,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B113" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E113" s="1">
         <v>0.85</v>
@@ -2757,10 +2748,10 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E114" s="1">
         <v>0.85</v>
@@ -2768,10 +2759,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B115" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E115" s="1">
         <v>0.85</v>
@@ -2779,10 +2770,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B116" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E116" s="1">
         <v>0.85</v>
@@ -2790,10 +2781,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B117" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E117" s="1">
         <v>0.85</v>
@@ -2801,10 +2792,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B118" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E118" s="1">
         <v>0.85</v>
@@ -2812,10 +2803,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B119" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E119" s="1">
         <v>0.85</v>
@@ -2823,10 +2814,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B120" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E120" s="1">
         <v>0.85</v>
@@ -2834,10 +2825,10 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B121" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E121" s="1">
         <v>0.85</v>
@@ -2845,10 +2836,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B122" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E122" s="1">
         <v>0.85</v>
@@ -2856,10 +2847,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E123" s="1">
         <v>0.85</v>
@@ -2867,10 +2858,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B124" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E124" s="1">
         <v>0.85</v>
@@ -2878,10 +2869,10 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B125" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E125" s="1">
         <v>0.85</v>
@@ -2889,10 +2880,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B126" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E126" s="1">
         <v>0.85</v>
@@ -2900,10 +2891,10 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B127" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E127" s="1">
         <v>0.85</v>
@@ -2911,10 +2902,10 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B128" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E128" s="1">
         <v>0.85</v>
@@ -2922,10 +2913,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B129" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E129" s="1">
         <v>0.85</v>
@@ -2933,10 +2924,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B130" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E130" s="1">
         <v>0.85</v>
@@ -2944,10 +2935,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B131" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E131" s="1">
         <v>0.85</v>
@@ -2955,10 +2946,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B132" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E132" s="1">
         <v>0.85</v>
@@ -2966,10 +2957,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B133" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E133" s="1">
         <v>0.85</v>
@@ -2977,10 +2968,10 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B134" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E134" s="1">
         <v>0.85</v>
@@ -2988,10 +2979,10 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B135" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E135" s="1">
         <v>0.85</v>
@@ -2999,10 +2990,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B136" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E136" s="1">
         <v>0.85</v>
@@ -3010,10 +3001,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B137" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E137" s="1">
         <v>0.85</v>
@@ -3021,10 +3012,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B138" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E138" s="1">
         <v>0.85</v>
@@ -3032,10 +3023,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B139" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E139" s="1">
         <v>0.85</v>
@@ -3043,10 +3034,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B140" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E140" s="1">
         <v>0.85</v>
@@ -3054,13 +3045,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B141" t="s">
+        <v>192</v>
+      </c>
+      <c r="C141" t="s">
         <v>193</v>
-      </c>
-      <c r="C141" t="s">
-        <v>194</v>
       </c>
       <c r="E141" s="1">
         <v>0.85</v>
@@ -3068,10 +3059,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>191</v>
+      </c>
+      <c r="B142" t="s">
         <v>192</v>
-      </c>
-      <c r="B142" t="s">
-        <v>193</v>
       </c>
       <c r="E142" s="1">
         <v>0.85</v>

</xml_diff>

<commit_message>
Add default description for loads in PDS (#2329)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="425">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1436,6 +1436,142 @@
   </si>
   <si>
     <t>Emergency Power Equipment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>住户配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>照明配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动力配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消防动力配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防排烟风机控制箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电表箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备配套控制箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隔离开关箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应急照明配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集中电源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消防照明配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消防照明配电箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电动机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防火卷帘控制盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电动排烟窗控制盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交流充电桩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非车载充电机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车道照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车位照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>正常照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机房照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机房照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>井道照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>室外照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>航空障碍灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灯具预留接线盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>疏散照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备用照明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>疏散指示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>插座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他用电设备</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交流充电桩预留</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1479,7 +1615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1490,6 +1626,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1771,15 +1910,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J285"/>
+  <dimension ref="A1:K285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
@@ -1789,9 +1928,10 @@
     <col min="8" max="8" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="24.77734375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1822,8 +1962,11 @@
       <c r="J1" s="4" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>234</v>
       </c>
@@ -1851,8 +1994,11 @@
       <c r="J2" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>236</v>
       </c>
@@ -1880,8 +2026,11 @@
       <c r="J3" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1912,26 +2061,23 @@
       <c r="J4" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>237</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>235</v>
-      </c>
       <c r="G5" s="3">
         <v>3</v>
       </c>
@@ -1944,20 +2090,29 @@
       <c r="J5" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F6" t="s">
+        <v>235</v>
+      </c>
       <c r="G6" s="3">
         <v>3</v>
       </c>
@@ -1970,8 +2125,11 @@
       <c r="J6" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -1996,8 +2154,11 @@
       <c r="J7" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2028,8 +2189,11 @@
       <c r="J8" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -2054,8 +2218,11 @@
       <c r="J9" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2086,8 +2253,11 @@
       <c r="J10" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -2112,8 +2282,11 @@
       <c r="J11" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2144,8 +2317,11 @@
       <c r="J12" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -2176,8 +2352,11 @@
       <c r="J13" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>242</v>
       </c>
@@ -2202,8 +2381,11 @@
       <c r="J14" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2234,8 +2416,11 @@
       <c r="J15" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>243</v>
       </c>
@@ -2260,8 +2445,11 @@
       <c r="J16" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2292,8 +2480,11 @@
       <c r="J17" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>244</v>
       </c>
@@ -2318,8 +2509,11 @@
       <c r="J18" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2350,8 +2544,11 @@
       <c r="J19" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2382,8 +2579,11 @@
       <c r="J20" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>245</v>
       </c>
@@ -2408,8 +2608,11 @@
       <c r="J21" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -2440,8 +2643,11 @@
       <c r="J22" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>246</v>
       </c>
@@ -2466,8 +2672,11 @@
       <c r="J23" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2486,8 +2695,11 @@
       <c r="I24" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>247</v>
       </c>
@@ -2506,8 +2718,11 @@
       <c r="I25" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2526,8 +2741,11 @@
       <c r="I26" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>248</v>
       </c>
@@ -2546,8 +2764,11 @@
       <c r="I27" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2569,8 +2790,11 @@
       <c r="I28" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>249</v>
       </c>
@@ -2592,8 +2816,11 @@
       <c r="I29" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2618,8 +2845,11 @@
       <c r="I30" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>188</v>
       </c>
@@ -2638,8 +2868,11 @@
       <c r="I31" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2658,8 +2891,11 @@
       <c r="I32" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>206</v>
       </c>
@@ -2678,8 +2914,11 @@
       <c r="I33" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>202</v>
       </c>
@@ -2698,8 +2937,11 @@
       <c r="I34" s="3">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>203</v>
       </c>
@@ -2721,8 +2963,11 @@
       <c r="J35" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -2753,8 +2998,11 @@
       <c r="J36" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>250</v>
       </c>
@@ -2779,8 +3027,11 @@
       <c r="J37" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -2811,8 +3062,11 @@
       <c r="J38" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>251</v>
       </c>
@@ -2837,8 +3091,11 @@
       <c r="J39" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2863,8 +3120,11 @@
       <c r="J40" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -2889,8 +3149,11 @@
       <c r="J41" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2915,22 +3178,25 @@
       <c r="J42" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>252</v>
       </c>
       <c r="B43" t="s">
         <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>210</v>
+        <v>18</v>
       </c>
       <c r="G43" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H43" s="3">
         <v>1</v>
@@ -2941,10 +3207,13 @@
       <c r="J43" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B44" t="s">
         <v>32</v>
@@ -2967,10 +3236,13 @@
       <c r="J44" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B45" t="s">
         <v>32</v>
@@ -2993,10 +3265,13 @@
       <c r="J45" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>254</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
@@ -3005,10 +3280,10 @@
         <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="G46" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H46" s="3">
         <v>1</v>
@@ -3019,8 +3294,11 @@
       <c r="J46" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -3045,8 +3323,11 @@
       <c r="J47" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>256</v>
       </c>
@@ -3071,8 +3352,11 @@
       <c r="J48" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>257</v>
       </c>
@@ -3097,8 +3381,11 @@
       <c r="J49" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>258</v>
       </c>
@@ -3123,8 +3410,11 @@
       <c r="J50" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>259</v>
       </c>
@@ -3132,7 +3422,7 @@
         <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>18</v>
@@ -3149,8 +3439,11 @@
       <c r="J51" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -3172,8 +3465,11 @@
       <c r="J52" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>292</v>
       </c>
@@ -3195,8 +3491,11 @@
       <c r="J53" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>68</v>
       </c>
@@ -3224,8 +3523,11 @@
       <c r="J54" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -3247,8 +3549,11 @@
       <c r="J55" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -3270,8 +3575,11 @@
       <c r="J56" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -3296,8 +3604,11 @@
       <c r="J57" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -3322,8 +3633,11 @@
       <c r="J58" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3345,8 +3659,11 @@
       <c r="J59" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -3368,8 +3685,11 @@
       <c r="J60" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3394,8 +3714,11 @@
       <c r="J61" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -3417,8 +3740,11 @@
       <c r="J62" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -3440,8 +3766,11 @@
       <c r="J63" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -3463,8 +3792,11 @@
       <c r="J64" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3486,8 +3818,11 @@
       <c r="J65" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -3509,8 +3844,11 @@
       <c r="J66" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3532,8 +3870,11 @@
       <c r="J67" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -3555,8 +3896,11 @@
       <c r="J68" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>96</v>
       </c>
@@ -3578,8 +3922,11 @@
       <c r="J69" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>97</v>
       </c>
@@ -3601,8 +3948,11 @@
       <c r="J70" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -3624,8 +3974,11 @@
       <c r="J71" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>99</v>
       </c>
@@ -3647,8 +4000,11 @@
       <c r="J72" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -3670,8 +4026,11 @@
       <c r="J73" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3693,8 +4052,11 @@
       <c r="J74" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -3716,8 +4078,11 @@
       <c r="J75" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -3742,8 +4107,11 @@
       <c r="J76" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>93</v>
       </c>
@@ -3768,8 +4136,11 @@
       <c r="J77" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -3791,8 +4162,11 @@
       <c r="J78" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -3817,8 +4191,11 @@
       <c r="J79" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>100</v>
       </c>
@@ -3840,8 +4217,11 @@
       <c r="J80" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -3863,8 +4243,11 @@
       <c r="J81" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
@@ -3886,8 +4269,11 @@
       <c r="J82" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K82" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -3909,8 +4295,11 @@
       <c r="J83" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3932,8 +4321,11 @@
       <c r="J84" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -3958,8 +4350,11 @@
       <c r="J85" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -3981,8 +4376,11 @@
       <c r="J86" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -4004,8 +4402,11 @@
       <c r="J87" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -4027,8 +4428,11 @@
       <c r="J88" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K88" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -4050,8 +4454,11 @@
       <c r="J89" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -4073,8 +4480,11 @@
       <c r="J90" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -4099,8 +4509,11 @@
       <c r="J91" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K91" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -4122,8 +4535,11 @@
       <c r="J92" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K92" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -4145,8 +4561,11 @@
       <c r="J93" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -4171,8 +4590,11 @@
       <c r="J94" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -4197,8 +4619,11 @@
       <c r="J95" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -4226,8 +4651,11 @@
       <c r="J96" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -4252,8 +4680,11 @@
       <c r="J97" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -4281,8 +4712,11 @@
       <c r="J98" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -4307,8 +4741,11 @@
       <c r="J99" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K99" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -4333,8 +4770,11 @@
       <c r="J100" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K100" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -4359,8 +4799,11 @@
       <c r="J101" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -4385,8 +4828,11 @@
       <c r="J102" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K102" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -4411,8 +4857,11 @@
       <c r="J103" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K103" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -4437,8 +4886,11 @@
       <c r="J104" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K104" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -4463,8 +4915,11 @@
       <c r="J105" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K105" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -4489,8 +4944,11 @@
       <c r="J106" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K106" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -4515,8 +4973,11 @@
       <c r="J107" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K107" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -4541,8 +5002,11 @@
       <c r="J108" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K108" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -4567,8 +5031,11 @@
       <c r="J109" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K109" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -4593,8 +5060,11 @@
       <c r="J110" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K110" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -4619,8 +5089,11 @@
       <c r="J111" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K111" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -4645,8 +5118,11 @@
       <c r="J112" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K112" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -4671,8 +5147,11 @@
       <c r="J113" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K113" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -4697,8 +5176,11 @@
       <c r="J114" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K114" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -4723,8 +5205,11 @@
       <c r="J115" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K115" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -4749,8 +5234,11 @@
       <c r="J116" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K116" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -4775,8 +5263,11 @@
       <c r="J117" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K117" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -4801,8 +5292,11 @@
       <c r="J118" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K118" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -4827,8 +5321,11 @@
       <c r="J119" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K119" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -4853,8 +5350,11 @@
       <c r="J120" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K120" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -4879,8 +5379,11 @@
       <c r="J121" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K121" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>356</v>
       </c>
@@ -4905,8 +5408,11 @@
       <c r="J122" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K122" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -4931,8 +5437,11 @@
       <c r="J123" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K123" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -4957,8 +5466,11 @@
       <c r="J124" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K124" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -4983,8 +5495,11 @@
       <c r="J125" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K125" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -5009,8 +5524,11 @@
       <c r="J126" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K126" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -5035,8 +5553,11 @@
       <c r="J127" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K127" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -5061,8 +5582,11 @@
       <c r="J128" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K128" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -5087,8 +5611,11 @@
       <c r="J129" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K129" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -5113,8 +5640,11 @@
       <c r="J130" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K130" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -5142,8 +5672,11 @@
       <c r="J131" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K131" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -5168,8 +5701,11 @@
       <c r="J132" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K132" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -5197,8 +5733,11 @@
       <c r="J133" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K133" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -5223,8 +5762,11 @@
       <c r="J134" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K134" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -5252,8 +5794,11 @@
       <c r="J135" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K135" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -5281,8 +5826,11 @@
       <c r="J136" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K136" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -5310,8 +5858,11 @@
       <c r="J137" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K137" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -5339,8 +5890,11 @@
       <c r="J138" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K138" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -5368,8 +5922,11 @@
       <c r="J139" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K139" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>291</v>
       </c>
@@ -5391,8 +5948,11 @@
       <c r="J140" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K140" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>293</v>
       </c>
@@ -5414,8 +5974,11 @@
       <c r="J141" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K141" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>294</v>
       </c>
@@ -5437,8 +6000,11 @@
       <c r="J142" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K142" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>295</v>
       </c>
@@ -5463,8 +6029,11 @@
       <c r="J143" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K143" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>296</v>
       </c>
@@ -5489,8 +6058,11 @@
       <c r="J144" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K144" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>298</v>
       </c>
@@ -5512,8 +6084,11 @@
       <c r="J145" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K145" s="5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>299</v>
       </c>
@@ -5535,8 +6110,11 @@
       <c r="J146" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K146" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>297</v>
       </c>
@@ -5561,8 +6139,11 @@
       <c r="J147" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K147" s="5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>303</v>
       </c>
@@ -5584,8 +6165,11 @@
       <c r="J148" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K148" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>300</v>
       </c>
@@ -5607,8 +6191,11 @@
       <c r="J149" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K149" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>304</v>
       </c>
@@ -5630,8 +6217,11 @@
       <c r="J150" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K150" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>301</v>
       </c>
@@ -5653,8 +6243,11 @@
       <c r="J151" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K151" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>305</v>
       </c>
@@ -5676,8 +6269,11 @@
       <c r="J152" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K152" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -5699,8 +6295,11 @@
       <c r="J153" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K153" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>318</v>
       </c>
@@ -5722,8 +6321,11 @@
       <c r="J154" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K154" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>319</v>
       </c>
@@ -5745,8 +6347,11 @@
       <c r="J155" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K155" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>320</v>
       </c>
@@ -5768,8 +6373,11 @@
       <c r="J156" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K156" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>321</v>
       </c>
@@ -5791,8 +6399,11 @@
       <c r="J157" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K157" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>322</v>
       </c>
@@ -5814,8 +6425,11 @@
       <c r="J158" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K158" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>311</v>
       </c>
@@ -5837,8 +6451,11 @@
       <c r="J159" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K159" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>306</v>
       </c>
@@ -5860,8 +6477,11 @@
       <c r="J160" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K160" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>307</v>
       </c>
@@ -5883,8 +6503,11 @@
       <c r="J161" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K161" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>310</v>
       </c>
@@ -5909,8 +6532,11 @@
       <c r="J162" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K162" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>316</v>
       </c>
@@ -5935,8 +6561,11 @@
       <c r="J163" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K163" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>308</v>
       </c>
@@ -5958,8 +6587,11 @@
       <c r="J164" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K164" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>309</v>
       </c>
@@ -5984,8 +6616,11 @@
       <c r="J165" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K165" s="5" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>323</v>
       </c>
@@ -6007,8 +6642,11 @@
       <c r="J166" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K166" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>314</v>
       </c>
@@ -6030,8 +6668,11 @@
       <c r="J167" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K167" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>315</v>
       </c>
@@ -6053,8 +6694,11 @@
       <c r="J168" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K168" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>313</v>
       </c>
@@ -6076,8 +6720,11 @@
       <c r="J169" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K169" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>312</v>
       </c>
@@ -6099,8 +6746,11 @@
       <c r="J170" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K170" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>317</v>
       </c>
@@ -6125,8 +6775,11 @@
       <c r="J171" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K171" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>328</v>
       </c>
@@ -6148,8 +6801,11 @@
       <c r="J172" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K172" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>329</v>
       </c>
@@ -6171,8 +6827,11 @@
       <c r="J173" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K173" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>325</v>
       </c>
@@ -6194,8 +6853,11 @@
       <c r="J174" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K174" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>326</v>
       </c>
@@ -6217,8 +6879,11 @@
       <c r="J175" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K175" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>327</v>
       </c>
@@ -6240,8 +6905,11 @@
       <c r="J176" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K176" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>324</v>
       </c>
@@ -6266,8 +6934,11 @@
       <c r="J177" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K177" s="5" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>330</v>
       </c>
@@ -6289,8 +6960,11 @@
       <c r="J178" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K178" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>331</v>
       </c>
@@ -6312,8 +6986,11 @@
       <c r="J179" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K179" s="5" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>332</v>
       </c>
@@ -6335,8 +7012,11 @@
       <c r="J180" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K180" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>333</v>
       </c>
@@ -6358,8 +7038,11 @@
       <c r="J181" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K181" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>334</v>
       </c>
@@ -6384,8 +7067,11 @@
       <c r="J182" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K182" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>335</v>
       </c>
@@ -6407,8 +7093,11 @@
       <c r="J183" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K183" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>336</v>
       </c>
@@ -6433,8 +7122,11 @@
       <c r="J184" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K184" s="5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>337</v>
       </c>
@@ -6459,8 +7151,11 @@
       <c r="J185" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K185" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>341</v>
       </c>
@@ -6485,8 +7180,11 @@
       <c r="J186" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K186" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>338</v>
       </c>
@@ -6511,8 +7209,11 @@
       <c r="J187" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K187" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>342</v>
       </c>
@@ -6537,8 +7238,11 @@
       <c r="J188" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K188" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>345</v>
       </c>
@@ -6563,8 +7267,11 @@
       <c r="J189" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K189" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>346</v>
       </c>
@@ -6589,8 +7296,11 @@
       <c r="J190" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K190" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>363</v>
       </c>
@@ -6615,8 +7325,11 @@
       <c r="J191" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K191" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>364</v>
       </c>
@@ -6641,8 +7354,11 @@
       <c r="J192" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K192" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>365</v>
       </c>
@@ -6667,8 +7383,11 @@
       <c r="J193" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K193" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>366</v>
       </c>
@@ -6693,8 +7412,11 @@
       <c r="J194" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K194" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>339</v>
       </c>
@@ -6719,8 +7441,11 @@
       <c r="J195" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K195" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>343</v>
       </c>
@@ -6745,8 +7470,11 @@
       <c r="J196" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K196" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>340</v>
       </c>
@@ -6771,8 +7499,11 @@
       <c r="J197" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K197" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>344</v>
       </c>
@@ -6797,8 +7528,11 @@
       <c r="J198" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K198" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>347</v>
       </c>
@@ -6823,8 +7557,11 @@
       <c r="J199" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K199" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>348</v>
       </c>
@@ -6849,8 +7586,11 @@
       <c r="J200" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K200" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>349</v>
       </c>
@@ -6875,8 +7615,11 @@
       <c r="J201" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K201" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>351</v>
       </c>
@@ -6901,8 +7644,11 @@
       <c r="J202" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K202" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>353</v>
       </c>
@@ -6927,8 +7673,11 @@
       <c r="J203" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K203" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>350</v>
       </c>
@@ -6953,8 +7702,11 @@
       <c r="J204" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K204" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>352</v>
       </c>
@@ -6979,8 +7731,11 @@
       <c r="J205" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K205" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>354</v>
       </c>
@@ -7005,8 +7760,11 @@
       <c r="J206" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K206" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -7031,8 +7789,11 @@
       <c r="J207" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K207" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>358</v>
       </c>
@@ -7057,8 +7818,11 @@
       <c r="J208" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K208" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>359</v>
       </c>
@@ -7083,8 +7847,11 @@
       <c r="J209" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K209" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>360</v>
       </c>
@@ -7109,8 +7876,11 @@
       <c r="J210" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K210" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>361</v>
       </c>
@@ -7135,8 +7905,11 @@
       <c r="J211" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K211" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -7161,8 +7934,11 @@
       <c r="J212" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K212" s="5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>367</v>
       </c>
@@ -7187,8 +7963,11 @@
       <c r="J213" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K213" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>368</v>
       </c>
@@ -7213,8 +7992,11 @@
       <c r="J214" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K214" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>369</v>
       </c>
@@ -7239,8 +8021,11 @@
       <c r="J215" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K215" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>370</v>
       </c>
@@ -7265,8 +8050,11 @@
       <c r="J216" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K216" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>375</v>
       </c>
@@ -7291,8 +8079,11 @@
       <c r="J217" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K217" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>371</v>
       </c>
@@ -7317,8 +8108,11 @@
       <c r="J218" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K218" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>376</v>
       </c>
@@ -7343,8 +8137,11 @@
       <c r="J219" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K219" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>372</v>
       </c>
@@ -7369,8 +8166,11 @@
       <c r="J220" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K220" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>377</v>
       </c>
@@ -7395,8 +8195,11 @@
       <c r="J221" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K221" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>373</v>
       </c>
@@ -7421,8 +8224,11 @@
       <c r="J222" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K222" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>378</v>
       </c>
@@ -7447,8 +8253,11 @@
       <c r="J223" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K223" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>374</v>
       </c>
@@ -7473,8 +8282,11 @@
       <c r="J224" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K224" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>379</v>
       </c>
@@ -7499,8 +8311,11 @@
       <c r="J225" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K225" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>168</v>
       </c>
@@ -7525,8 +8340,11 @@
       <c r="J226" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K226" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>157</v>
       </c>
@@ -7551,8 +8369,11 @@
       <c r="J227" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K227" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>169</v>
       </c>
@@ -7577,8 +8398,11 @@
       <c r="J228" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K228" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>170</v>
       </c>
@@ -7603,8 +8427,11 @@
       <c r="J229" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K229" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>174</v>
       </c>
@@ -7629,8 +8456,11 @@
       <c r="J230" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K230" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>175</v>
       </c>
@@ -7655,8 +8485,11 @@
       <c r="J231" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K231" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>176</v>
       </c>
@@ -7681,8 +8514,11 @@
       <c r="J232" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K232" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>289</v>
       </c>
@@ -7707,8 +8543,11 @@
       <c r="J233" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K233" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>167</v>
       </c>
@@ -7733,8 +8572,11 @@
       <c r="J234" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K234" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>172</v>
       </c>
@@ -7759,8 +8601,11 @@
       <c r="J235" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K235" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>171</v>
       </c>
@@ -7785,8 +8630,11 @@
       <c r="J236" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K236" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>173</v>
       </c>
@@ -7811,8 +8659,11 @@
       <c r="J237" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K237" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>178</v>
       </c>
@@ -7837,8 +8688,11 @@
       <c r="J238" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K238" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>179</v>
       </c>
@@ -7863,8 +8717,11 @@
       <c r="J239" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K239" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>177</v>
       </c>
@@ -7889,8 +8746,11 @@
       <c r="J240" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K240" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>158</v>
       </c>
@@ -7915,8 +8775,11 @@
       <c r="J241" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K241" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>159</v>
       </c>
@@ -7941,8 +8804,11 @@
       <c r="J242" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K242" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>160</v>
       </c>
@@ -7967,8 +8833,11 @@
       <c r="J243" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K243" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>161</v>
       </c>
@@ -7993,8 +8862,11 @@
       <c r="J244" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K244" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>181</v>
       </c>
@@ -8019,8 +8891,11 @@
       <c r="J245" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K245" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>182</v>
       </c>
@@ -8045,8 +8920,11 @@
       <c r="J246" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K246" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>162</v>
       </c>
@@ -8071,8 +8949,11 @@
       <c r="J247" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K247" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>180</v>
       </c>
@@ -8097,8 +8978,11 @@
       <c r="J248" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K248" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>163</v>
       </c>
@@ -8123,8 +9007,11 @@
       <c r="J249" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K249" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>164</v>
       </c>
@@ -8149,8 +9036,11 @@
       <c r="J250" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K250" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>165</v>
       </c>
@@ -8175,8 +9065,11 @@
       <c r="J251" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K251" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>166</v>
       </c>
@@ -8201,8 +9094,11 @@
       <c r="J252" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K252" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>183</v>
       </c>
@@ -8227,8 +9123,11 @@
       <c r="J253" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K253" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>184</v>
       </c>
@@ -8253,8 +9152,11 @@
       <c r="J254" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K254" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>185</v>
       </c>
@@ -8279,8 +9181,11 @@
       <c r="J255" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K255" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>271</v>
       </c>
@@ -8305,8 +9210,11 @@
       <c r="J256" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K256" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>260</v>
       </c>
@@ -8331,8 +9239,11 @@
       <c r="J257" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K257" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>272</v>
       </c>
@@ -8357,8 +9268,11 @@
       <c r="J258" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K258" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>273</v>
       </c>
@@ -8383,8 +9297,11 @@
       <c r="J259" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K259" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>277</v>
       </c>
@@ -8409,8 +9326,11 @@
       <c r="J260" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K260" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>278</v>
       </c>
@@ -8435,8 +9355,11 @@
       <c r="J261" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K261" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>279</v>
       </c>
@@ -8461,8 +9384,11 @@
       <c r="J262" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K262" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>290</v>
       </c>
@@ -8487,8 +9413,11 @@
       <c r="J263" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K263" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>270</v>
       </c>
@@ -8513,8 +9442,11 @@
       <c r="J264" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K264" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>275</v>
       </c>
@@ -8539,8 +9471,11 @@
       <c r="J265" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K265" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>274</v>
       </c>
@@ -8565,8 +9500,11 @@
       <c r="J266" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K266" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>276</v>
       </c>
@@ -8591,8 +9529,11 @@
       <c r="J267" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K267" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>281</v>
       </c>
@@ -8617,8 +9558,11 @@
       <c r="J268" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K268" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>282</v>
       </c>
@@ -8643,8 +9587,11 @@
       <c r="J269" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K269" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>280</v>
       </c>
@@ -8669,8 +9616,11 @@
       <c r="J270" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K270" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>261</v>
       </c>
@@ -8695,8 +9645,11 @@
       <c r="J271" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K271" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>262</v>
       </c>
@@ -8721,8 +9674,11 @@
       <c r="J272" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K272" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>263</v>
       </c>
@@ -8747,8 +9703,11 @@
       <c r="J273" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K273" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>264</v>
       </c>
@@ -8773,8 +9732,11 @@
       <c r="J274" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K274" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>284</v>
       </c>
@@ -8799,8 +9761,11 @@
       <c r="J275" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K275" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>285</v>
       </c>
@@ -8825,8 +9790,11 @@
       <c r="J276" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K276" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>265</v>
       </c>
@@ -8851,8 +9819,11 @@
       <c r="J277" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K277" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>283</v>
       </c>
@@ -8877,8 +9848,11 @@
       <c r="J278" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K278" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>266</v>
       </c>
@@ -8903,8 +9877,11 @@
       <c r="J279" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K279" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>267</v>
       </c>
@@ -8929,8 +9906,11 @@
       <c r="J280" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K280" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>268</v>
       </c>
@@ -8955,8 +9935,11 @@
       <c r="J281" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K281" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>269</v>
       </c>
@@ -8981,8 +9964,11 @@
       <c r="J282" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K282" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>286</v>
       </c>
@@ -9007,8 +9993,11 @@
       <c r="J283" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K283" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>287</v>
       </c>
@@ -9033,8 +10022,11 @@
       <c r="J284" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K284" s="5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>288</v>
       </c>
@@ -9058,6 +10050,9 @@
       </c>
       <c r="J285" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="K285" s="5" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cable laying method form support file (#2411)
* Fix a bug

* Add cable laying method form support file

Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="432">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1572,6 +1572,34 @@
   </si>
   <si>
     <t>交流充电桩预留</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cable laying method 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cable laying method 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1615,7 +1643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1628,6 +1656,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1910,10 +1941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K285"/>
+  <dimension ref="A1:M285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1923,15 +1954,17 @@
     <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="3" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="4"/>
     <col min="11" max="11" width="24.77734375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1965,8 +1998,14 @@
       <c r="K1" s="5" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>234</v>
       </c>
@@ -1997,8 +2036,14 @@
       <c r="K2" s="5" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>236</v>
       </c>
@@ -2029,8 +2074,14 @@
       <c r="K3" s="5" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2064,8 +2115,14 @@
       <c r="K4" s="5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>237</v>
       </c>
@@ -2093,8 +2150,14 @@
       <c r="K5" s="5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2128,8 +2191,14 @@
       <c r="K6" s="5" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -2157,8 +2226,14 @@
       <c r="K7" s="5" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2192,8 +2267,14 @@
       <c r="K8" s="5" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -2221,8 +2302,14 @@
       <c r="K9" s="5" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2256,8 +2343,14 @@
       <c r="K10" s="5" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -2285,8 +2378,14 @@
       <c r="K11" s="5" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2320,8 +2419,14 @@
       <c r="K12" s="5" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -2355,8 +2460,14 @@
       <c r="K13" s="5" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>242</v>
       </c>
@@ -2384,8 +2495,14 @@
       <c r="K14" s="5" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2413,14 +2530,17 @@
       <c r="I15" s="3">
         <v>0.8</v>
       </c>
-      <c r="J15" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="K15" s="5" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>243</v>
       </c>
@@ -2442,14 +2562,17 @@
       <c r="I16" s="3">
         <v>0.8</v>
       </c>
-      <c r="J16" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="K16" s="5" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2477,14 +2600,17 @@
       <c r="I17" s="3">
         <v>0.85</v>
       </c>
-      <c r="J17" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="K17" s="5" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>244</v>
       </c>
@@ -2506,14 +2632,17 @@
       <c r="I18" s="3">
         <v>0.85</v>
       </c>
-      <c r="J18" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="K18" s="5" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2541,14 +2670,17 @@
       <c r="I19" s="3">
         <v>0.85</v>
       </c>
-      <c r="J19" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="K19" s="5" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2582,8 +2714,14 @@
       <c r="K20" s="5" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>245</v>
       </c>
@@ -2611,8 +2749,14 @@
       <c r="K21" s="5" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -2646,8 +2790,14 @@
       <c r="K22" s="5" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>246</v>
       </c>
@@ -2675,8 +2825,14 @@
       <c r="K23" s="5" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2698,8 +2854,11 @@
       <c r="K24" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>247</v>
       </c>
@@ -2721,8 +2880,11 @@
       <c r="K25" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2744,8 +2906,11 @@
       <c r="K26" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>248</v>
       </c>
@@ -2767,8 +2932,11 @@
       <c r="K27" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2793,8 +2961,14 @@
       <c r="K28" s="5" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>249</v>
       </c>
@@ -2819,8 +2993,14 @@
       <c r="K29" s="5" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2848,8 +3028,14 @@
       <c r="K30" s="5" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>188</v>
       </c>
@@ -2871,8 +3057,11 @@
       <c r="K31" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2894,8 +3083,11 @@
       <c r="K32" s="5" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>206</v>
       </c>
@@ -2917,8 +3109,14 @@
       <c r="K33" s="5" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>202</v>
       </c>
@@ -2940,8 +3138,11 @@
       <c r="K34" s="5" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>203</v>
       </c>
@@ -2960,14 +3161,14 @@
       <c r="I35" s="3">
         <v>0.85</v>
       </c>
-      <c r="J35" s="4" t="b">
-        <v>0</v>
-      </c>
       <c r="K35" s="5" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -3001,8 +3202,14 @@
       <c r="K36" s="5" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>250</v>
       </c>
@@ -3030,8 +3237,14 @@
       <c r="K37" s="5" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -3065,8 +3278,14 @@
       <c r="K38" s="5" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>251</v>
       </c>
@@ -3094,8 +3313,14 @@
       <c r="K39" s="5" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3123,8 +3348,14 @@
       <c r="K40" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3152,8 +3383,14 @@
       <c r="K41" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -3181,8 +3418,14 @@
       <c r="K42" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>252</v>
       </c>
@@ -3210,8 +3453,14 @@
       <c r="K43" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>253</v>
       </c>
@@ -3239,8 +3488,14 @@
       <c r="K44" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>254</v>
       </c>
@@ -3268,8 +3523,14 @@
       <c r="K45" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -3297,8 +3558,14 @@
       <c r="K46" s="5" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -3326,8 +3593,14 @@
       <c r="K47" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>256</v>
       </c>
@@ -3355,8 +3628,14 @@
       <c r="K48" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M48" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>257</v>
       </c>
@@ -3384,8 +3663,14 @@
       <c r="K49" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>258</v>
       </c>
@@ -3413,8 +3698,14 @@
       <c r="K50" s="5" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>259</v>
       </c>
@@ -3442,8 +3733,14 @@
       <c r="K51" s="5" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -3468,8 +3765,11 @@
       <c r="K52" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>292</v>
       </c>
@@ -3494,8 +3794,11 @@
       <c r="K53" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>68</v>
       </c>
@@ -3526,8 +3829,11 @@
       <c r="K54" s="5" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -3552,8 +3858,11 @@
       <c r="K55" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -3578,8 +3887,11 @@
       <c r="K56" s="5" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -3607,8 +3919,11 @@
       <c r="K57" s="5" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -3636,8 +3951,11 @@
       <c r="K58" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3662,8 +3980,11 @@
       <c r="K59" s="5" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -3688,8 +4009,11 @@
       <c r="K60" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3717,8 +4041,11 @@
       <c r="K61" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -3743,8 +4070,11 @@
       <c r="K62" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -3769,8 +4099,11 @@
       <c r="K63" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -3795,8 +4128,11 @@
       <c r="K64" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3821,8 +4157,11 @@
       <c r="K65" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -3847,8 +4186,11 @@
       <c r="K66" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3873,8 +4215,11 @@
       <c r="K67" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -3899,8 +4244,11 @@
       <c r="K68" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>96</v>
       </c>
@@ -3925,8 +4273,11 @@
       <c r="K69" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>97</v>
       </c>
@@ -3951,8 +4302,11 @@
       <c r="K70" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -3977,8 +4331,11 @@
       <c r="K71" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>99</v>
       </c>
@@ -4003,8 +4360,11 @@
       <c r="K72" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -4029,8 +4389,11 @@
       <c r="K73" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -4055,8 +4418,11 @@
       <c r="K74" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -4081,8 +4447,11 @@
       <c r="K75" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4110,8 +4479,11 @@
       <c r="K76" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>93</v>
       </c>
@@ -4139,8 +4511,11 @@
       <c r="K77" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -4165,8 +4540,14 @@
       <c r="K78" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M78" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -4194,8 +4575,14 @@
       <c r="K79" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M79" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>100</v>
       </c>
@@ -4220,8 +4607,14 @@
       <c r="K80" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M80" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -4246,8 +4639,14 @@
       <c r="K81" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M81" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
@@ -4272,8 +4671,14 @@
       <c r="K82" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M82" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -4298,8 +4703,11 @@
       <c r="K83" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L83" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -4324,8 +4732,11 @@
       <c r="K84" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -4353,8 +4764,11 @@
       <c r="K85" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -4379,8 +4793,11 @@
       <c r="K86" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -4405,8 +4822,11 @@
       <c r="K87" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -4431,8 +4851,11 @@
       <c r="K88" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -4457,8 +4880,11 @@
       <c r="K89" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -4483,8 +4909,11 @@
       <c r="K90" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -4512,8 +4941,14 @@
       <c r="K91" s="5" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M91" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -4538,8 +4973,14 @@
       <c r="K92" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L92" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M92" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -4564,8 +5005,14 @@
       <c r="K93" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L93" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -4593,8 +5040,14 @@
       <c r="K94" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L94" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M94" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -4622,8 +5075,14 @@
       <c r="K95" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L95" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M95" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -4654,8 +5113,14 @@
       <c r="K96" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L96" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M96" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -4683,8 +5148,11 @@
       <c r="K97" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L97" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -4715,8 +5183,11 @@
       <c r="K98" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L98" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -4744,8 +5215,14 @@
       <c r="K99" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L99" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M99" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -4773,8 +5250,14 @@
       <c r="K100" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L100" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M100" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -4802,8 +5285,11 @@
       <c r="K101" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L101" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -4831,8 +5317,11 @@
       <c r="K102" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L102" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -4860,8 +5349,14 @@
       <c r="K103" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L103" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M103" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -4889,8 +5384,14 @@
       <c r="K104" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L104" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M104" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -4918,8 +5419,14 @@
       <c r="K105" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L105" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M105" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -4947,8 +5454,11 @@
       <c r="K106" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L106" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -4976,8 +5486,14 @@
       <c r="K107" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L107" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M107" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -5005,8 +5521,11 @@
       <c r="K108" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L108" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -5034,8 +5553,14 @@
       <c r="K109" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L109" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M109" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -5063,8 +5588,11 @@
       <c r="K110" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L110" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -5092,8 +5620,14 @@
       <c r="K111" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L111" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M111" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -5121,8 +5655,11 @@
       <c r="K112" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L112" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -5150,8 +5687,11 @@
       <c r="K113" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L113" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -5179,8 +5719,11 @@
       <c r="K114" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L114" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -5208,8 +5751,14 @@
       <c r="K115" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L115" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M115" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -5237,8 +5786,11 @@
       <c r="K116" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L116" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -5266,8 +5818,11 @@
       <c r="K117" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L117" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -5295,8 +5850,14 @@
       <c r="K118" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L118" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M118" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -5324,8 +5885,11 @@
       <c r="K119" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L119" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -5353,8 +5917,11 @@
       <c r="K120" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L120" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -5382,8 +5949,11 @@
       <c r="K121" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L121" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>356</v>
       </c>
@@ -5411,8 +5981,14 @@
       <c r="K122" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L122" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M122" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -5440,8 +6016,14 @@
       <c r="K123" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L123" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M123" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -5469,8 +6051,14 @@
       <c r="K124" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L124" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M124" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -5498,8 +6086,14 @@
       <c r="K125" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L125" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M125" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -5527,8 +6121,14 @@
       <c r="K126" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L126" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M126" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -5556,8 +6156,14 @@
       <c r="K127" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L127" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M127" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -5585,8 +6191,14 @@
       <c r="K128" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L128" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M128" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -5614,8 +6226,14 @@
       <c r="K129" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L129" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M129" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -5643,8 +6261,11 @@
       <c r="K130" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L130" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -5675,8 +6296,11 @@
       <c r="K131" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L131" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -5704,8 +6328,14 @@
       <c r="K132" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L132" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M132" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -5736,8 +6366,14 @@
       <c r="K133" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L133" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M133" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -5765,8 +6401,14 @@
       <c r="K134" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L134" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M134" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -5797,8 +6439,14 @@
       <c r="K135" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L135" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M135" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -5829,8 +6477,11 @@
       <c r="K136" s="5" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L136" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -5861,8 +6512,11 @@
       <c r="K137" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L137" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -5893,8 +6547,11 @@
       <c r="K138" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L138" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -5925,8 +6582,11 @@
       <c r="K139" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L139" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>291</v>
       </c>
@@ -5951,8 +6611,11 @@
       <c r="K140" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L140" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>293</v>
       </c>
@@ -5977,8 +6640,11 @@
       <c r="K141" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L141" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>294</v>
       </c>
@@ -6003,8 +6669,11 @@
       <c r="K142" s="5" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L142" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>295</v>
       </c>
@@ -6032,8 +6701,11 @@
       <c r="K143" s="5" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L143" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>296</v>
       </c>
@@ -6061,8 +6733,11 @@
       <c r="K144" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L144" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>298</v>
       </c>
@@ -6087,8 +6762,11 @@
       <c r="K145" s="5" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L145" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>299</v>
       </c>
@@ -6113,8 +6791,11 @@
       <c r="K146" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L146" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>297</v>
       </c>
@@ -6142,8 +6823,11 @@
       <c r="K147" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L147" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>303</v>
       </c>
@@ -6168,8 +6852,11 @@
       <c r="K148" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L148" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>300</v>
       </c>
@@ -6194,8 +6881,11 @@
       <c r="K149" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L149" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>304</v>
       </c>
@@ -6220,8 +6910,11 @@
       <c r="K150" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L150" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>301</v>
       </c>
@@ -6246,8 +6939,11 @@
       <c r="K151" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L151" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>305</v>
       </c>
@@ -6272,8 +6968,11 @@
       <c r="K152" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L152" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -6298,8 +6997,11 @@
       <c r="K153" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L153" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>318</v>
       </c>
@@ -6324,8 +7026,11 @@
       <c r="K154" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L154" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>319</v>
       </c>
@@ -6350,8 +7055,11 @@
       <c r="K155" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L155" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>320</v>
       </c>
@@ -6376,8 +7084,11 @@
       <c r="K156" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L156" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>321</v>
       </c>
@@ -6402,8 +7113,11 @@
       <c r="K157" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L157" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>322</v>
       </c>
@@ -6428,8 +7142,11 @@
       <c r="K158" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L158" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>311</v>
       </c>
@@ -6454,8 +7171,11 @@
       <c r="K159" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L159" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>306</v>
       </c>
@@ -6480,8 +7200,11 @@
       <c r="K160" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L160" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>307</v>
       </c>
@@ -6506,8 +7229,11 @@
       <c r="K161" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L161" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>310</v>
       </c>
@@ -6535,8 +7261,11 @@
       <c r="K162" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L162" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>316</v>
       </c>
@@ -6564,8 +7293,11 @@
       <c r="K163" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L163" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>308</v>
       </c>
@@ -6590,8 +7322,14 @@
       <c r="K164" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L164" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M164" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>309</v>
       </c>
@@ -6619,8 +7357,14 @@
       <c r="K165" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L165" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M165" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>323</v>
       </c>
@@ -6645,8 +7389,14 @@
       <c r="K166" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L166" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M166" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>314</v>
       </c>
@@ -6671,8 +7421,14 @@
       <c r="K167" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L167" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M167" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>315</v>
       </c>
@@ -6697,8 +7453,14 @@
       <c r="K168" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L168" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M168" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>313</v>
       </c>
@@ -6723,8 +7485,11 @@
       <c r="K169" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L169" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>312</v>
       </c>
@@ -6749,8 +7514,11 @@
       <c r="K170" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L170" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>317</v>
       </c>
@@ -6778,8 +7546,11 @@
       <c r="K171" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L171" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>328</v>
       </c>
@@ -6804,8 +7575,11 @@
       <c r="K172" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L172" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>329</v>
       </c>
@@ -6830,8 +7604,11 @@
       <c r="K173" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L173" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>325</v>
       </c>
@@ -6856,8 +7633,11 @@
       <c r="K174" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L174" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>326</v>
       </c>
@@ -6882,8 +7662,11 @@
       <c r="K175" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L175" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>327</v>
       </c>
@@ -6908,8 +7691,11 @@
       <c r="K176" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L176" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>324</v>
       </c>
@@ -6937,8 +7723,14 @@
       <c r="K177" s="5" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L177" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M177" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>330</v>
       </c>
@@ -6963,8 +7755,14 @@
       <c r="K178" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L178" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M178" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>331</v>
       </c>
@@ -6989,8 +7787,14 @@
       <c r="K179" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L179" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M179" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>332</v>
       </c>
@@ -7015,8 +7819,14 @@
       <c r="K180" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L180" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M180" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>333</v>
       </c>
@@ -7041,8 +7851,14 @@
       <c r="K181" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L181" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M181" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>334</v>
       </c>
@@ -7070,8 +7886,14 @@
       <c r="K182" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L182" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M182" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>335</v>
       </c>
@@ -7096,8 +7918,11 @@
       <c r="K183" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L183" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>336</v>
       </c>
@@ -7125,8 +7950,11 @@
       <c r="K184" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L184" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>337</v>
       </c>
@@ -7154,8 +7982,14 @@
       <c r="K185" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L185" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M185" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>341</v>
       </c>
@@ -7183,8 +8017,14 @@
       <c r="K186" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L186" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M186" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>338</v>
       </c>
@@ -7212,8 +8052,11 @@
       <c r="K187" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L187" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>342</v>
       </c>
@@ -7241,8 +8084,11 @@
       <c r="K188" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L188" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>345</v>
       </c>
@@ -7270,8 +8116,14 @@
       <c r="K189" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L189" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M189" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>346</v>
       </c>
@@ -7299,8 +8151,14 @@
       <c r="K190" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L190" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M190" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>363</v>
       </c>
@@ -7328,8 +8186,14 @@
       <c r="K191" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L191" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M191" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>364</v>
       </c>
@@ -7357,8 +8221,11 @@
       <c r="K192" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L192" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>365</v>
       </c>
@@ -7386,8 +8253,14 @@
       <c r="K193" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L193" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M193" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>366</v>
       </c>
@@ -7415,8 +8288,11 @@
       <c r="K194" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L194" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>339</v>
       </c>
@@ -7444,8 +8320,14 @@
       <c r="K195" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L195" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M195" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>343</v>
       </c>
@@ -7473,8 +8355,11 @@
       <c r="K196" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L196" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>340</v>
       </c>
@@ -7502,8 +8387,14 @@
       <c r="K197" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L197" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M197" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>344</v>
       </c>
@@ -7531,8 +8422,11 @@
       <c r="K198" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L198" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>347</v>
       </c>
@@ -7560,8 +8454,11 @@
       <c r="K199" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L199" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>348</v>
       </c>
@@ -7589,8 +8486,11 @@
       <c r="K200" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L200" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>349</v>
       </c>
@@ -7618,8 +8518,14 @@
       <c r="K201" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L201" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M201" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>351</v>
       </c>
@@ -7647,8 +8553,11 @@
       <c r="K202" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L202" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>353</v>
       </c>
@@ -7676,8 +8585,11 @@
       <c r="K203" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L203" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>350</v>
       </c>
@@ -7705,8 +8617,14 @@
       <c r="K204" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L204" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M204" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>352</v>
       </c>
@@ -7734,8 +8652,11 @@
       <c r="K205" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L205" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>354</v>
       </c>
@@ -7763,8 +8684,11 @@
       <c r="K206" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L206" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -7792,8 +8716,11 @@
       <c r="K207" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L207" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>358</v>
       </c>
@@ -7821,8 +8748,14 @@
       <c r="K208" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L208" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M208" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>359</v>
       </c>
@@ -7850,8 +8783,14 @@
       <c r="K209" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L209" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M209" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>360</v>
       </c>
@@ -7879,8 +8818,14 @@
       <c r="K210" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L210" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M210" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>361</v>
       </c>
@@ -7908,8 +8853,14 @@
       <c r="K211" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L211" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M211" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -7937,8 +8888,14 @@
       <c r="K212" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L212" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M212" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>367</v>
       </c>
@@ -7966,8 +8923,14 @@
       <c r="K213" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L213" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M213" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>368</v>
       </c>
@@ -7995,8 +8958,14 @@
       <c r="K214" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L214" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M214" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>369</v>
       </c>
@@ -8024,8 +8993,14 @@
       <c r="K215" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L215" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M215" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>370</v>
       </c>
@@ -8053,8 +9028,11 @@
       <c r="K216" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L216" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>375</v>
       </c>
@@ -8082,8 +9060,11 @@
       <c r="K217" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L217" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>371</v>
       </c>
@@ -8111,8 +9092,14 @@
       <c r="K218" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L218" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M218" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>376</v>
       </c>
@@ -8140,8 +9127,14 @@
       <c r="K219" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L219" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M219" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>372</v>
       </c>
@@ -8169,8 +9162,14 @@
       <c r="K220" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L220" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M220" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>377</v>
       </c>
@@ -8198,8 +9197,14 @@
       <c r="K221" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L221" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M221" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>373</v>
       </c>
@@ -8227,8 +9232,11 @@
       <c r="K222" s="5" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L222" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>378</v>
       </c>
@@ -8256,8 +9264,11 @@
       <c r="K223" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L223" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>374</v>
       </c>
@@ -8285,8 +9296,11 @@
       <c r="K224" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L224" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>379</v>
       </c>
@@ -8314,8 +9328,11 @@
       <c r="K225" s="5" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L225" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>168</v>
       </c>
@@ -8343,8 +9360,14 @@
       <c r="K226" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L226" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M226" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>157</v>
       </c>
@@ -8372,8 +9395,14 @@
       <c r="K227" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L227" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M227" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>169</v>
       </c>
@@ -8401,8 +9430,14 @@
       <c r="K228" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L228" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M228" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>170</v>
       </c>
@@ -8430,8 +9465,14 @@
       <c r="K229" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L229" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M229" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>174</v>
       </c>
@@ -8459,8 +9500,14 @@
       <c r="K230" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L230" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M230" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>175</v>
       </c>
@@ -8488,8 +9535,14 @@
       <c r="K231" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L231" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M231" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>176</v>
       </c>
@@ -8517,8 +9570,14 @@
       <c r="K232" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L232" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M232" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>289</v>
       </c>
@@ -8546,8 +9605,14 @@
       <c r="K233" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L233" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M233" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>167</v>
       </c>
@@ -8575,8 +9640,14 @@
       <c r="K234" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L234" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M234" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>172</v>
       </c>
@@ -8604,8 +9675,14 @@
       <c r="K235" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L235" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M235" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>171</v>
       </c>
@@ -8633,8 +9710,14 @@
       <c r="K236" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L236" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M236" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>173</v>
       </c>
@@ -8662,8 +9745,14 @@
       <c r="K237" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L237" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M237" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>178</v>
       </c>
@@ -8691,8 +9780,14 @@
       <c r="K238" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L238" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M238" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>179</v>
       </c>
@@ -8720,8 +9815,14 @@
       <c r="K239" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L239" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M239" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>177</v>
       </c>
@@ -8749,8 +9850,14 @@
       <c r="K240" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L240" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M240" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>158</v>
       </c>
@@ -8778,8 +9885,14 @@
       <c r="K241" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L241" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M241" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>159</v>
       </c>
@@ -8807,8 +9920,14 @@
       <c r="K242" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L242" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M242" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>160</v>
       </c>
@@ -8836,8 +9955,14 @@
       <c r="K243" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L243" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M243" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>161</v>
       </c>
@@ -8865,8 +9990,12 @@
       <c r="K244" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L244" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M244" s="6"/>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>181</v>
       </c>
@@ -8894,8 +10023,14 @@
       <c r="K245" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L245" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M245" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>182</v>
       </c>
@@ -8923,8 +10058,14 @@
       <c r="K246" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L246" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M246" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>162</v>
       </c>
@@ -8952,8 +10093,14 @@
       <c r="K247" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L247" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M247" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>180</v>
       </c>
@@ -8981,8 +10128,14 @@
       <c r="K248" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L248" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M248" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>163</v>
       </c>
@@ -9010,8 +10163,14 @@
       <c r="K249" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L249" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M249" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>164</v>
       </c>
@@ -9039,8 +10198,14 @@
       <c r="K250" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L250" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M250" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>165</v>
       </c>
@@ -9068,8 +10233,14 @@
       <c r="K251" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L251" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M251" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>166</v>
       </c>
@@ -9097,8 +10268,12 @@
       <c r="K252" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L252" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M252" s="6"/>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>183</v>
       </c>
@@ -9126,8 +10301,14 @@
       <c r="K253" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L253" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M253" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>184</v>
       </c>
@@ -9155,8 +10336,14 @@
       <c r="K254" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L254" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M254" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>185</v>
       </c>
@@ -9184,8 +10371,14 @@
       <c r="K255" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L255" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M255" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>271</v>
       </c>
@@ -9213,8 +10406,14 @@
       <c r="K256" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L256" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M256" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>260</v>
       </c>
@@ -9242,8 +10441,14 @@
       <c r="K257" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L257" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M257" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>272</v>
       </c>
@@ -9271,8 +10476,14 @@
       <c r="K258" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L258" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M258" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>273</v>
       </c>
@@ -9300,8 +10511,14 @@
       <c r="K259" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L259" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M259" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>277</v>
       </c>
@@ -9329,8 +10546,14 @@
       <c r="K260" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L260" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M260" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>278</v>
       </c>
@@ -9358,8 +10581,14 @@
       <c r="K261" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L261" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M261" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>279</v>
       </c>
@@ -9387,8 +10616,14 @@
       <c r="K262" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L262" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M262" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>290</v>
       </c>
@@ -9416,8 +10651,14 @@
       <c r="K263" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L263" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M263" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>270</v>
       </c>
@@ -9445,8 +10686,14 @@
       <c r="K264" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L264" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M264" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>275</v>
       </c>
@@ -9474,8 +10721,14 @@
       <c r="K265" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L265" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M265" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>274</v>
       </c>
@@ -9503,8 +10756,14 @@
       <c r="K266" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L266" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M266" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>276</v>
       </c>
@@ -9532,8 +10791,14 @@
       <c r="K267" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L267" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M267" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>281</v>
       </c>
@@ -9561,8 +10826,14 @@
       <c r="K268" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L268" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M268" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>282</v>
       </c>
@@ -9590,8 +10861,14 @@
       <c r="K269" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L269" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M269" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>280</v>
       </c>
@@ -9619,8 +10896,14 @@
       <c r="K270" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L270" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M270" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>261</v>
       </c>
@@ -9648,8 +10931,14 @@
       <c r="K271" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L271" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M271" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>262</v>
       </c>
@@ -9677,8 +10966,14 @@
       <c r="K272" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L272" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M272" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>263</v>
       </c>
@@ -9706,8 +11001,14 @@
       <c r="K273" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L273" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M273" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>264</v>
       </c>
@@ -9735,8 +11036,12 @@
       <c r="K274" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L274" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M274" s="6"/>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>284</v>
       </c>
@@ -9764,8 +11069,14 @@
       <c r="K275" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L275" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M275" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>285</v>
       </c>
@@ -9793,8 +11104,14 @@
       <c r="K276" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L276" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M276" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>265</v>
       </c>
@@ -9822,8 +11139,14 @@
       <c r="K277" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L277" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M277" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>283</v>
       </c>
@@ -9851,8 +11174,14 @@
       <c r="K278" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L278" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M278" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>266</v>
       </c>
@@ -9880,8 +11209,14 @@
       <c r="K279" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L279" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M279" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>267</v>
       </c>
@@ -9909,8 +11244,14 @@
       <c r="K280" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L280" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M280" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>268</v>
       </c>
@@ -9938,8 +11279,14 @@
       <c r="K281" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L281" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M281" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>269</v>
       </c>
@@ -9967,8 +11314,12 @@
       <c r="K282" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L282" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M282" s="6"/>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>286</v>
       </c>
@@ -9996,8 +11347,14 @@
       <c r="K283" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L283" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M283" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>287</v>
       </c>
@@ -10025,8 +11382,14 @@
       <c r="K284" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L284" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M284" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>288</v>
       </c>
@@ -10053,6 +11416,12 @@
       </c>
       <c r="K285" s="5" t="s">
         <v>422</v>
+      </c>
+      <c r="L285" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M285" s="5" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a bug in PDS (#2770)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Block" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="524">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1910,6 +1910,30 @@
   </si>
   <si>
     <t>Terminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BEMS100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电能表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BEMS110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BEMS120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>燃气表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2255,24 +2279,24 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="4"/>
-    <col min="11" max="11" width="24.77734375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="3" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.875" style="4"/>
+    <col min="11" max="11" width="24.75" style="5" customWidth="1"/>
+    <col min="12" max="12" width="21.875" style="5" customWidth="1"/>
+    <col min="13" max="13" width="21.625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2313,7 +2337,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>234</v>
       </c>
@@ -2351,7 +2375,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>236</v>
       </c>
@@ -2389,7 +2413,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2430,7 +2454,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>237</v>
       </c>
@@ -2465,7 +2489,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2506,7 +2530,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>238</v>
       </c>
@@ -2541,7 +2565,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2582,7 +2606,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -2617,7 +2641,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -2658,7 +2682,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -2693,7 +2717,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2734,7 +2758,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>241</v>
       </c>
@@ -2775,7 +2799,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>242</v>
       </c>
@@ -2810,7 +2834,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2851,7 +2875,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>243</v>
       </c>
@@ -2886,7 +2910,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2927,7 +2951,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>244</v>
       </c>
@@ -2962,7 +2986,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -3003,7 +3027,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -3044,7 +3068,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>245</v>
       </c>
@@ -3079,7 +3103,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -3120,7 +3144,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>246</v>
       </c>
@@ -3155,7 +3179,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -3181,7 +3205,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>247</v>
       </c>
@@ -3207,7 +3231,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3233,7 +3257,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>248</v>
       </c>
@@ -3259,7 +3283,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3291,7 +3315,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>249</v>
       </c>
@@ -3323,7 +3347,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3358,7 +3382,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>188</v>
       </c>
@@ -3384,7 +3408,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3410,7 +3434,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>206</v>
       </c>
@@ -3439,7 +3463,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>202</v>
       </c>
@@ -3465,7 +3489,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>203</v>
       </c>
@@ -3494,7 +3518,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -3535,7 +3559,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>250</v>
       </c>
@@ -3570,7 +3594,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -3611,7 +3635,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>251</v>
       </c>
@@ -3646,7 +3670,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3681,7 +3705,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3716,7 +3740,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -3751,7 +3775,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>252</v>
       </c>
@@ -3786,7 +3810,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>253</v>
       </c>
@@ -3821,7 +3845,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>254</v>
       </c>
@@ -3856,7 +3880,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -3891,7 +3915,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -3926,7 +3950,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>256</v>
       </c>
@@ -3961,7 +3985,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>257</v>
       </c>
@@ -3996,7 +4020,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>258</v>
       </c>
@@ -4031,7 +4055,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>259</v>
       </c>
@@ -4066,7 +4090,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -4095,7 +4119,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>292</v>
       </c>
@@ -4124,7 +4148,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>68</v>
       </c>
@@ -4159,7 +4183,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -4188,7 +4212,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -4217,7 +4241,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -4249,7 +4273,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -4281,7 +4305,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -4310,7 +4334,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -4339,7 +4363,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -4371,7 +4395,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -4400,7 +4424,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -4429,7 +4453,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -4458,7 +4482,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -4487,7 +4511,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -4516,7 +4540,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -4545,7 +4569,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -4574,7 +4598,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>96</v>
       </c>
@@ -4603,7 +4627,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>97</v>
       </c>
@@ -4632,7 +4656,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>98</v>
       </c>
@@ -4661,7 +4685,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>99</v>
       </c>
@@ -4690,7 +4714,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -4719,7 +4743,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -4748,7 +4772,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -4777,7 +4801,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4809,7 +4833,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>93</v>
       </c>
@@ -4841,7 +4865,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -4873,7 +4897,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -4908,7 +4932,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>100</v>
       </c>
@@ -4940,7 +4964,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -4972,7 +4996,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>92</v>
       </c>
@@ -5004,7 +5028,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -5033,7 +5057,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -5062,7 +5086,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -5094,7 +5118,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -5123,7 +5147,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -5152,7 +5176,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -5181,7 +5205,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -5210,7 +5234,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -5239,7 +5263,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -5274,7 +5298,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -5306,7 +5330,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -5338,7 +5362,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -5373,7 +5397,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -5408,7 +5432,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -5446,7 +5470,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -5478,7 +5502,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -5513,7 +5537,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -5548,7 +5572,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -5583,7 +5607,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -5615,7 +5639,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>118</v>
       </c>
@@ -5647,7 +5671,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>119</v>
       </c>
@@ -5682,7 +5706,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>120</v>
       </c>
@@ -5717,7 +5741,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>121</v>
       </c>
@@ -5752,7 +5776,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>122</v>
       </c>
@@ -5784,7 +5808,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -5819,7 +5843,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>124</v>
       </c>
@@ -5851,7 +5875,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>125</v>
       </c>
@@ -5886,7 +5910,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -5918,7 +5942,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -5953,7 +5977,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -5985,7 +6009,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -6017,7 +6041,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>130</v>
       </c>
@@ -6049,7 +6073,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>131</v>
       </c>
@@ -6084,7 +6108,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>132</v>
       </c>
@@ -6116,7 +6140,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>133</v>
       </c>
@@ -6148,7 +6172,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>134</v>
       </c>
@@ -6183,7 +6207,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -6215,7 +6239,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -6247,7 +6271,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>355</v>
       </c>
@@ -6279,7 +6303,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>356</v>
       </c>
@@ -6314,7 +6338,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -6349,7 +6373,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -6384,7 +6408,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -6419,7 +6443,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -6454,7 +6478,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -6489,7 +6513,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -6524,7 +6548,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -6559,7 +6583,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -6591,7 +6615,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -6626,7 +6650,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -6661,7 +6685,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -6699,7 +6723,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -6734,7 +6758,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -6772,7 +6796,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -6807,7 +6831,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -6842,7 +6866,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -6877,7 +6901,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -6912,7 +6936,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>291</v>
       </c>
@@ -6941,7 +6965,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>293</v>
       </c>
@@ -6970,7 +6994,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>294</v>
       </c>
@@ -6999,7 +7023,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>295</v>
       </c>
@@ -7031,7 +7055,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>296</v>
       </c>
@@ -7063,7 +7087,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>298</v>
       </c>
@@ -7092,7 +7116,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>299</v>
       </c>
@@ -7121,7 +7145,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>297</v>
       </c>
@@ -7153,7 +7177,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>303</v>
       </c>
@@ -7182,7 +7206,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>300</v>
       </c>
@@ -7211,7 +7235,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>304</v>
       </c>
@@ -7240,7 +7264,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>301</v>
       </c>
@@ -7269,7 +7293,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>305</v>
       </c>
@@ -7298,7 +7322,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>302</v>
       </c>
@@ -7327,7 +7351,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>318</v>
       </c>
@@ -7356,7 +7380,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>319</v>
       </c>
@@ -7385,7 +7409,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>320</v>
       </c>
@@ -7414,7 +7438,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>321</v>
       </c>
@@ -7443,7 +7467,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>322</v>
       </c>
@@ -7472,7 +7496,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>311</v>
       </c>
@@ -7501,7 +7525,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>306</v>
       </c>
@@ -7530,7 +7554,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>307</v>
       </c>
@@ -7559,7 +7583,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>310</v>
       </c>
@@ -7591,7 +7615,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>316</v>
       </c>
@@ -7623,7 +7647,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>308</v>
       </c>
@@ -7655,7 +7679,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>309</v>
       </c>
@@ -7690,7 +7714,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>323</v>
       </c>
@@ -7722,7 +7746,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>314</v>
       </c>
@@ -7754,7 +7778,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>315</v>
       </c>
@@ -7786,7 +7810,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>313</v>
       </c>
@@ -7815,7 +7839,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>312</v>
       </c>
@@ -7844,7 +7868,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>317</v>
       </c>
@@ -7876,7 +7900,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>328</v>
       </c>
@@ -7905,7 +7929,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>329</v>
       </c>
@@ -7934,7 +7958,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>325</v>
       </c>
@@ -7963,7 +7987,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>326</v>
       </c>
@@ -7992,7 +8016,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>327</v>
       </c>
@@ -8021,7 +8045,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>324</v>
       </c>
@@ -8056,7 +8080,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>330</v>
       </c>
@@ -8088,7 +8112,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>331</v>
       </c>
@@ -8120,7 +8144,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>332</v>
       </c>
@@ -8152,7 +8176,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>333</v>
       </c>
@@ -8184,7 +8208,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>334</v>
       </c>
@@ -8219,7 +8243,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>335</v>
       </c>
@@ -8248,7 +8272,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>336</v>
       </c>
@@ -8280,7 +8304,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>337</v>
       </c>
@@ -8315,7 +8339,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>341</v>
       </c>
@@ -8350,7 +8374,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>338</v>
       </c>
@@ -8382,7 +8406,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>342</v>
       </c>
@@ -8414,7 +8438,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>345</v>
       </c>
@@ -8449,7 +8473,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>346</v>
       </c>
@@ -8484,7 +8508,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>363</v>
       </c>
@@ -8519,7 +8543,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>364</v>
       </c>
@@ -8551,7 +8575,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>365</v>
       </c>
@@ -8586,7 +8610,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>366</v>
       </c>
@@ -8618,7 +8642,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>339</v>
       </c>
@@ -8653,7 +8677,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>343</v>
       </c>
@@ -8685,7 +8709,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>340</v>
       </c>
@@ -8720,7 +8744,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>344</v>
       </c>
@@ -8752,7 +8776,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>347</v>
       </c>
@@ -8784,7 +8808,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>348</v>
       </c>
@@ -8816,7 +8840,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>349</v>
       </c>
@@ -8851,7 +8875,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>351</v>
       </c>
@@ -8883,7 +8907,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>353</v>
       </c>
@@ -8915,7 +8939,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>350</v>
       </c>
@@ -8950,7 +8974,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>352</v>
       </c>
@@ -8982,7 +9006,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>354</v>
       </c>
@@ -9014,7 +9038,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -9046,7 +9070,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>358</v>
       </c>
@@ -9081,7 +9105,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>359</v>
       </c>
@@ -9116,7 +9140,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>360</v>
       </c>
@@ -9151,7 +9175,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>361</v>
       </c>
@@ -9186,7 +9210,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>362</v>
       </c>
@@ -9221,7 +9245,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>367</v>
       </c>
@@ -9256,7 +9280,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>368</v>
       </c>
@@ -9291,7 +9315,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>369</v>
       </c>
@@ -9326,7 +9350,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>370</v>
       </c>
@@ -9358,7 +9382,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>375</v>
       </c>
@@ -9390,7 +9414,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>371</v>
       </c>
@@ -9425,7 +9449,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>376</v>
       </c>
@@ -9460,7 +9484,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>372</v>
       </c>
@@ -9495,7 +9519,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>377</v>
       </c>
@@ -9530,7 +9554,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>373</v>
       </c>
@@ -9562,7 +9586,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>378</v>
       </c>
@@ -9594,7 +9618,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>374</v>
       </c>
@@ -9626,7 +9650,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>379</v>
       </c>
@@ -9658,7 +9682,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>168</v>
       </c>
@@ -9693,7 +9717,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>157</v>
       </c>
@@ -9728,7 +9752,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>169</v>
       </c>
@@ -9763,7 +9787,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>170</v>
       </c>
@@ -9798,7 +9822,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>174</v>
       </c>
@@ -9833,7 +9857,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>175</v>
       </c>
@@ -9868,7 +9892,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>176</v>
       </c>
@@ -9903,7 +9927,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>289</v>
       </c>
@@ -9938,7 +9962,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>167</v>
       </c>
@@ -9973,7 +9997,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>172</v>
       </c>
@@ -10008,7 +10032,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>171</v>
       </c>
@@ -10043,7 +10067,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>173</v>
       </c>
@@ -10078,7 +10102,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>178</v>
       </c>
@@ -10113,7 +10137,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>179</v>
       </c>
@@ -10148,7 +10172,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>177</v>
       </c>
@@ -10183,7 +10207,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>158</v>
       </c>
@@ -10218,7 +10242,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>159</v>
       </c>
@@ -10253,7 +10277,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>160</v>
       </c>
@@ -10288,7 +10312,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>161</v>
       </c>
@@ -10321,7 +10345,7 @@
       </c>
       <c r="M244" s="6"/>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>181</v>
       </c>
@@ -10356,7 +10380,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>182</v>
       </c>
@@ -10391,7 +10415,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>162</v>
       </c>
@@ -10426,7 +10450,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>180</v>
       </c>
@@ -10461,7 +10485,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>163</v>
       </c>
@@ -10496,7 +10520,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>164</v>
       </c>
@@ -10531,7 +10555,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>165</v>
       </c>
@@ -10566,7 +10590,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>166</v>
       </c>
@@ -10599,7 +10623,7 @@
       </c>
       <c r="M252" s="6"/>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>183</v>
       </c>
@@ -10634,7 +10658,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>184</v>
       </c>
@@ -10669,7 +10693,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>185</v>
       </c>
@@ -10704,7 +10728,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>271</v>
       </c>
@@ -10739,7 +10763,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>260</v>
       </c>
@@ -10774,7 +10798,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>272</v>
       </c>
@@ -10809,7 +10833,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>273</v>
       </c>
@@ -10844,7 +10868,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>277</v>
       </c>
@@ -10879,7 +10903,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>278</v>
       </c>
@@ -10914,7 +10938,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>279</v>
       </c>
@@ -10949,7 +10973,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>290</v>
       </c>
@@ -10984,7 +11008,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>270</v>
       </c>
@@ -11019,7 +11043,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>275</v>
       </c>
@@ -11054,7 +11078,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>274</v>
       </c>
@@ -11089,7 +11113,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>276</v>
       </c>
@@ -11124,7 +11148,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>281</v>
       </c>
@@ -11159,7 +11183,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>282</v>
       </c>
@@ -11194,7 +11218,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>280</v>
       </c>
@@ -11229,7 +11253,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>261</v>
       </c>
@@ -11264,7 +11288,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>262</v>
       </c>
@@ -11299,7 +11323,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>263</v>
       </c>
@@ -11334,7 +11358,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>264</v>
       </c>
@@ -11367,7 +11391,7 @@
       </c>
       <c r="M274" s="6"/>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>284</v>
       </c>
@@ -11402,7 +11426,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>285</v>
       </c>
@@ -11437,7 +11461,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>265</v>
       </c>
@@ -11472,7 +11496,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>283</v>
       </c>
@@ -11507,7 +11531,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>266</v>
       </c>
@@ -11542,7 +11566,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>267</v>
       </c>
@@ -11577,7 +11601,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>268</v>
       </c>
@@ -11612,7 +11636,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>269</v>
       </c>
@@ -11645,7 +11669,7 @@
       </c>
       <c r="M282" s="6"/>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>286</v>
       </c>
@@ -11680,7 +11704,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>287</v>
       </c>
@@ -11715,7 +11739,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>288</v>
       </c>
@@ -11765,14 +11789,14 @@
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" width="27.625" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -11783,7 +11807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -11794,7 +11818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -11805,7 +11829,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -11816,7 +11840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -11827,7 +11851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -11838,7 +11862,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>386</v>
       </c>
@@ -11849,7 +11873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -11860,7 +11884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -11871,7 +11895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -11882,7 +11906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>380</v>
       </c>
@@ -11893,7 +11917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>381</v>
       </c>
@@ -11904,7 +11928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>382</v>
       </c>
@@ -11915,7 +11939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -11926,7 +11950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>385</v>
       </c>
@@ -11937,7 +11961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -11948,7 +11972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -11959,7 +11983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -11967,7 +11991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>383</v>
       </c>
@@ -11975,7 +11999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>384</v>
       </c>
@@ -11986,7 +12010,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>387</v>
       </c>
@@ -12002,19 +12026,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12028,7 +12054,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>433</v>
       </c>
@@ -12039,7 +12065,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>439</v>
       </c>
@@ -12050,7 +12076,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>451</v>
       </c>
@@ -12061,7 +12087,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>452</v>
       </c>
@@ -12072,7 +12098,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>453</v>
       </c>
@@ -12083,7 +12109,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>436</v>
       </c>
@@ -12094,7 +12120,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>435</v>
       </c>
@@ -12105,7 +12131,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>437</v>
       </c>
@@ -12116,7 +12142,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>438</v>
       </c>
@@ -12127,7 +12153,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>447</v>
       </c>
@@ -12138,7 +12164,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>448</v>
       </c>
@@ -12149,7 +12175,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>440</v>
       </c>
@@ -12160,7 +12186,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>441</v>
       </c>
@@ -12171,7 +12197,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>442</v>
       </c>
@@ -12182,7 +12208,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>463</v>
       </c>
@@ -12193,7 +12219,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>464</v>
       </c>
@@ -12204,177 +12230,177 @@
         <v>461</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>476</v>
+        <v>518</v>
       </c>
       <c r="C18" t="s">
         <v>434</v>
       </c>
       <c r="D18" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>478</v>
+        <v>520</v>
       </c>
       <c r="C19" t="s">
         <v>434</v>
       </c>
       <c r="D19" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>466</v>
+        <v>522</v>
       </c>
       <c r="C20" t="s">
         <v>434</v>
       </c>
       <c r="D20" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="C21" t="s">
         <v>434</v>
       </c>
       <c r="D21" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="C22" t="s">
         <v>434</v>
       </c>
       <c r="D22" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="C23" t="s">
         <v>434</v>
       </c>
       <c r="D23" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C24" t="s">
         <v>434</v>
       </c>
       <c r="D24" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C25" t="s">
         <v>434</v>
       </c>
       <c r="D25" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C26" t="s">
         <v>434</v>
       </c>
       <c r="D26" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>473</v>
+      </c>
+      <c r="C27" t="s">
+        <v>434</v>
+      </c>
+      <c r="D27" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>474</v>
+      </c>
+      <c r="C28" t="s">
+        <v>434</v>
+      </c>
+      <c r="D28" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>465</v>
+      </c>
+      <c r="C29" t="s">
+        <v>434</v>
+      </c>
+      <c r="D29" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>455</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>456</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>457</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>479</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>457</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>480</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>457</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>483</v>
-      </c>
-      <c r="C30" t="s">
-        <v>485</v>
-      </c>
-      <c r="D30" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>486</v>
-      </c>
-      <c r="C31" t="s">
-        <v>485</v>
-      </c>
-      <c r="D31" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>487</v>
-      </c>
-      <c r="C32" t="s">
-        <v>517</v>
-      </c>
-      <c r="D32" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>489</v>
       </c>
       <c r="C33" t="s">
         <v>485</v>
@@ -12383,9 +12409,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C34" t="s">
         <v>485</v>
@@ -12394,20 +12420,20 @@
         <v>484</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C35" t="s">
-        <v>485</v>
+        <v>517</v>
       </c>
       <c r="D35" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C36" t="s">
         <v>485</v>
@@ -12416,9 +12442,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C37" t="s">
         <v>485</v>
@@ -12427,9 +12453,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C38" t="s">
         <v>485</v>
@@ -12438,9 +12464,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C39" t="s">
         <v>485</v>
@@ -12449,9 +12475,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C40" t="s">
         <v>485</v>
@@ -12460,9 +12486,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C41" t="s">
         <v>485</v>
@@ -12471,9 +12497,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C42" t="s">
         <v>485</v>
@@ -12482,9 +12508,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C43" t="s">
         <v>485</v>
@@ -12493,9 +12519,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C44" t="s">
         <v>485</v>
@@ -12504,9 +12530,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C45" t="s">
         <v>485</v>
@@ -12515,9 +12541,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="C46" t="s">
         <v>485</v>
@@ -12526,9 +12552,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C47" t="s">
         <v>485</v>
@@ -12537,9 +12563,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C48" t="s">
         <v>485</v>
@@ -12548,9 +12574,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C49" t="s">
         <v>485</v>
@@ -12559,9 +12585,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C50" t="s">
         <v>485</v>
@@ -12570,9 +12596,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C51" t="s">
         <v>485</v>
@@ -12581,9 +12607,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="C52" t="s">
         <v>485</v>
@@ -12592,9 +12618,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="C53" t="s">
         <v>485</v>
@@ -12603,9 +12629,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="C54" t="s">
         <v>485</v>
@@ -12614,9 +12640,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="C55" t="s">
         <v>485</v>
@@ -12625,9 +12651,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="C56" t="s">
         <v>485</v>
@@ -12636,9 +12662,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="C57" t="s">
         <v>485</v>
@@ -12647,9 +12673,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C58" t="s">
         <v>485</v>
@@ -12658,9 +12684,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C59" t="s">
         <v>485</v>
@@ -12669,14 +12695,47 @@
         <v>484</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="C60" t="s">
         <v>485</v>
       </c>
       <c r="D60" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>510</v>
+      </c>
+      <c r="C61" t="s">
+        <v>485</v>
+      </c>
+      <c r="D61" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>511</v>
+      </c>
+      <c r="C62" t="s">
+        <v>485</v>
+      </c>
+      <c r="D62" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>515</v>
+      </c>
+      <c r="C63" t="s">
+        <v>485</v>
+      </c>
+      <c r="D63" t="s">
         <v>484</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merge loads in different storeys (#3113)
* code optimization

* Update the config file

* Merge loads in different storeys

Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Block" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="527">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1934,6 +1934,18 @@
   </si>
   <si>
     <t>燃气表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emergency Power Equipment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire Emergency Lighting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFAS23-3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2277,8 +2289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2695,7 +2707,7 @@
         <v>63</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>390</v>
+        <v>524</v>
       </c>
       <c r="G11" s="3">
         <v>3</v>
@@ -6386,7 +6398,7 @@
         <v>193</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>212</v>
+        <v>525</v>
       </c>
       <c r="G124" s="3">
         <v>1</v>
@@ -12028,10 +12040,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12267,7 +12279,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>476</v>
+        <v>526</v>
       </c>
       <c r="C21" t="s">
         <v>434</v>
@@ -12278,7 +12290,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C22" t="s">
         <v>434</v>
@@ -12289,51 +12301,51 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="C23" t="s">
         <v>434</v>
       </c>
       <c r="D23" t="s">
-        <v>467</v>
+        <v>477</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C24" t="s">
         <v>434</v>
       </c>
       <c r="D24" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C25" t="s">
         <v>434</v>
       </c>
       <c r="D25" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C26" t="s">
         <v>434</v>
       </c>
       <c r="D26" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C27" t="s">
         <v>434</v>
@@ -12344,7 +12356,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C28" t="s">
         <v>434</v>
@@ -12355,65 +12367,65 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="C29" t="s">
         <v>434</v>
       </c>
       <c r="D29" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>455</v>
-      </c>
-      <c r="B30" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="C30" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="D30" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>479</v>
+        <v>455</v>
+      </c>
+      <c r="B31" t="s">
+        <v>456</v>
       </c>
       <c r="C31" t="s">
         <v>457</v>
       </c>
       <c r="D31" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C32" t="s">
         <v>457</v>
       </c>
       <c r="D32" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C33" t="s">
-        <v>485</v>
+        <v>457</v>
       </c>
       <c r="D33" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C34" t="s">
         <v>485</v>
@@ -12424,10 +12436,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C35" t="s">
-        <v>517</v>
+        <v>485</v>
       </c>
       <c r="D35" t="s">
         <v>484</v>
@@ -12435,10 +12447,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C36" t="s">
-        <v>485</v>
+        <v>517</v>
       </c>
       <c r="D36" t="s">
         <v>484</v>
@@ -12446,7 +12458,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C37" t="s">
         <v>485</v>
@@ -12457,7 +12469,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C38" t="s">
         <v>485</v>
@@ -12468,7 +12480,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C39" t="s">
         <v>485</v>
@@ -12479,7 +12491,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C40" t="s">
         <v>485</v>
@@ -12490,7 +12502,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C41" t="s">
         <v>485</v>
@@ -12501,7 +12513,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C42" t="s">
         <v>485</v>
@@ -12512,7 +12524,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C43" t="s">
         <v>485</v>
@@ -12523,7 +12535,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C44" t="s">
         <v>485</v>
@@ -12534,7 +12546,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C45" t="s">
         <v>485</v>
@@ -12545,7 +12557,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C46" t="s">
         <v>485</v>
@@ -12556,7 +12568,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C47" t="s">
         <v>485</v>
@@ -12567,7 +12579,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C48" t="s">
         <v>485</v>
@@ -12578,7 +12590,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="C49" t="s">
         <v>485</v>
@@ -12589,7 +12601,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C50" t="s">
         <v>485</v>
@@ -12600,7 +12612,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="C51" t="s">
         <v>485</v>
@@ -12611,7 +12623,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C52" t="s">
         <v>485</v>
@@ -12622,7 +12634,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C53" t="s">
         <v>485</v>
@@ -12633,7 +12645,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="C54" t="s">
         <v>485</v>
@@ -12644,7 +12656,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C55" t="s">
         <v>485</v>
@@ -12655,7 +12667,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="C56" t="s">
         <v>485</v>
@@ -12666,7 +12678,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C57" t="s">
         <v>485</v>
@@ -12677,7 +12689,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C58" t="s">
         <v>485</v>
@@ -12688,7 +12700,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="C59" t="s">
         <v>485</v>
@@ -12699,7 +12711,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C60" t="s">
         <v>485</v>
@@ -12710,7 +12722,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C61" t="s">
         <v>485</v>
@@ -12721,7 +12733,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C62" t="s">
         <v>485</v>
@@ -12732,12 +12744,23 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="C63" t="s">
         <v>485</v>
       </c>
       <c r="D63" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>515</v>
+      </c>
+      <c r="C64" t="s">
+        <v>485</v>
+      </c>
+      <c r="D64" t="s">
         <v>484</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PDS bugs fixing (#3139)
Co-authored-by: 刘潘 <liupan1@thape.com.cn>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/平面关注对象.xlsx
+++ b/AutoLoader/Contents/Support/平面关注对象.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="Block" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="529">
   <si>
     <t>Block</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1946,6 +1946,14 @@
   </si>
   <si>
     <t>E-BFAS23-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI-负载标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E-BFAS820</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2287,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M285"/>
+  <dimension ref="A1:M286"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3534,58 +3542,52 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>527</v>
       </c>
       <c r="B36" t="s">
-        <v>216</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="F36" t="s">
-        <v>235</v>
+        <v>18</v>
       </c>
       <c r="G36" s="3">
         <v>3</v>
       </c>
       <c r="H36" s="3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I36" s="3">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="J36" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="L36" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>250</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>216</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
       </c>
+      <c r="D37" t="s">
+        <v>34</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="F37" t="s">
+        <v>235</v>
+      </c>
       <c r="G37" s="3">
         <v>3</v>
       </c>
@@ -3610,23 +3612,17 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s">
         <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="F38" t="s">
-        <v>235</v>
-      </c>
       <c r="G38" s="3">
         <v>3</v>
       </c>
@@ -3640,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>427</v>
@@ -3651,7 +3647,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>251</v>
+        <v>528</v>
       </c>
       <c r="B39" t="s">
         <v>32</v>
@@ -3659,9 +3655,15 @@
       <c r="C39" t="s">
         <v>35</v>
       </c>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>390</v>
       </c>
+      <c r="F39" t="s">
+        <v>235</v>
+      </c>
       <c r="G39" s="3">
         <v>3</v>
       </c>
@@ -3686,31 +3688,31 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>251</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>210</v>
+        <v>390</v>
       </c>
       <c r="G40" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
       </c>
       <c r="I40" s="3">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="J40" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>427</v>
@@ -3721,7 +3723,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
@@ -3756,7 +3758,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
@@ -3791,7 +3793,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>32</v>
@@ -3800,7 +3802,7 @@
         <v>40</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="G43" s="3">
         <v>1</v>
@@ -3826,7 +3828,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B44" t="s">
         <v>32</v>
@@ -3861,7 +3863,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B45" t="s">
         <v>32</v>
@@ -3896,7 +3898,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>254</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
@@ -3905,10 +3907,10 @@
         <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>210</v>
+        <v>18</v>
       </c>
       <c r="G46" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H46" s="3">
         <v>1</v>
@@ -3920,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>427</v>
@@ -3931,16 +3933,16 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>255</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="G47" s="3">
         <v>3</v>
@@ -3955,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>408</v>
+        <v>424</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>427</v>
@@ -3966,7 +3968,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B48" t="s">
         <v>32</v>
@@ -4001,7 +4003,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B49" t="s">
         <v>32</v>
@@ -4036,7 +4038,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B50" t="s">
         <v>32</v>
@@ -4071,13 +4073,13 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B51" t="s">
         <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>18</v>
@@ -4095,60 +4097,66 @@
         <v>0</v>
       </c>
       <c r="K51" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="3">
+        <v>3</v>
+      </c>
+      <c r="H52" s="3">
+        <v>1</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="J52" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="L51" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="L52" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>195</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>197</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F52" t="s">
-        <v>199</v>
-      </c>
-      <c r="G52" s="3">
-        <v>1</v>
-      </c>
-      <c r="H52" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="I52" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="J52" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" t="s">
-        <v>191</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>211</v>
       </c>
+      <c r="F53" t="s">
+        <v>199</v>
+      </c>
       <c r="G53" s="3">
         <v>1</v>
       </c>
@@ -4162,7 +4170,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L53" s="5" t="s">
         <v>427</v>
@@ -4170,7 +4178,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
         <v>191</v>
@@ -4191,7 +4199,7 @@
         <v>0</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>427</v>
@@ -4199,13 +4207,13 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>292</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
         <v>191</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>20</v>
+        <v>211</v>
       </c>
       <c r="G55" s="3">
         <v>1</v>
@@ -4228,13 +4236,13 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>292</v>
       </c>
       <c r="B56" t="s">
         <v>191</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>211</v>
+        <v>20</v>
       </c>
       <c r="G56" s="3">
         <v>1</v>
@@ -4249,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="L56" s="5" t="s">
         <v>427</v>
@@ -4257,13 +4265,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
         <v>191</v>
-      </c>
-      <c r="C57" t="s">
-        <v>217</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>211</v>
@@ -4281,7 +4286,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>427</v>
@@ -4289,13 +4294,13 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
         <v>191</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>211</v>
@@ -4313,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L58" s="5" t="s">
         <v>427</v>
@@ -4321,10 +4326,13 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
         <v>191</v>
+      </c>
+      <c r="C59" t="s">
+        <v>196</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>211</v>
@@ -4342,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L59" s="5" t="s">
         <v>427</v>
@@ -4350,7 +4358,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" t="s">
         <v>191</v>
@@ -4371,7 +4379,7 @@
         <v>0</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L60" s="5" t="s">
         <v>427</v>
@@ -4379,13 +4387,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
         <v>191</v>
-      </c>
-      <c r="C61" t="s">
-        <v>196</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>211</v>
@@ -4411,10 +4416,13 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
         <v>191</v>
+      </c>
+      <c r="C62" t="s">
+        <v>196</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>211</v>
@@ -4432,7 +4440,7 @@
         <v>0</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="L62" s="5" t="s">
         <v>427</v>
@@ -4440,7 +4448,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
         <v>191</v>
@@ -4469,7 +4477,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
         <v>191</v>
@@ -4498,7 +4506,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
         <v>191</v>
@@ -4527,7 +4535,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
         <v>191</v>
@@ -4556,7 +4564,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B67" t="s">
         <v>191</v>
@@ -4585,7 +4593,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
         <v>191</v>
@@ -4614,7 +4622,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
         <v>191</v>
@@ -4643,7 +4651,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B70" t="s">
         <v>191</v>
@@ -4672,7 +4680,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" t="s">
         <v>191</v>
@@ -4701,7 +4709,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B72" t="s">
         <v>191</v>
@@ -4730,7 +4738,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
         <v>191</v>
@@ -4759,7 +4767,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
         <v>191</v>
@@ -4788,7 +4796,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B75" t="s">
         <v>191</v>
@@ -4817,13 +4825,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
         <v>191</v>
-      </c>
-      <c r="D76" t="s">
-        <v>87</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>211</v>
@@ -4849,13 +4854,13 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
         <v>191</v>
       </c>
-      <c r="C77" t="s">
-        <v>196</v>
+      <c r="D77" t="s">
+        <v>87</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>211</v>
@@ -4873,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>427</v>
@@ -4881,10 +4886,13 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B78" t="s">
         <v>191</v>
+      </c>
+      <c r="C78" t="s">
+        <v>196</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>211</v>
@@ -4902,24 +4910,18 @@
         <v>0</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="L78" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="M78" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
         <v>191</v>
-      </c>
-      <c r="C79" t="s">
-        <v>218</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>211</v>
@@ -4937,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="L79" s="5" t="s">
         <v>427</v>
@@ -4948,10 +4950,13 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B80" t="s">
         <v>191</v>
+      </c>
+      <c r="C80" t="s">
+        <v>218</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>211</v>
@@ -4969,7 +4974,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>427</v>
@@ -4980,7 +4985,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
         <v>191</v>
@@ -5012,7 +5017,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" t="s">
         <v>191</v>
@@ -5044,7 +5049,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>191</v>
@@ -5070,10 +5075,13 @@
       <c r="L83" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M83" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" t="s">
         <v>191</v>
@@ -5102,13 +5110,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B85" t="s">
         <v>191</v>
-      </c>
-      <c r="C85" t="s">
-        <v>196</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>211</v>
@@ -5126,7 +5131,7 @@
         <v>0</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>427</v>
@@ -5134,10 +5139,13 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B86" t="s">
         <v>191</v>
+      </c>
+      <c r="C86" t="s">
+        <v>196</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>211</v>
@@ -5155,7 +5163,7 @@
         <v>0</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>427</v>
@@ -5163,7 +5171,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B87" t="s">
         <v>191</v>
@@ -5192,7 +5200,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B88" t="s">
         <v>191</v>
@@ -5221,7 +5229,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B89" t="s">
         <v>191</v>
@@ -5250,7 +5258,7 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B90" t="s">
         <v>191</v>
@@ -5279,13 +5287,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B91" t="s">
         <v>191</v>
-      </c>
-      <c r="C91" t="s">
-        <v>198</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>211</v>
@@ -5303,21 +5308,21 @@
         <v>0</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="M91" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B92" t="s">
         <v>191</v>
+      </c>
+      <c r="C92" t="s">
+        <v>198</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>211</v>
@@ -5335,7 +5340,7 @@
         <v>0</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="L92" s="5" t="s">
         <v>427</v>
@@ -5346,7 +5351,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B93" t="s">
         <v>191</v>
@@ -5378,13 +5383,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B94" t="s">
         <v>191</v>
-      </c>
-      <c r="D94" t="s">
-        <v>113</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>211</v>
@@ -5402,18 +5404,18 @@
         <v>0</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L94" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M94" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B95" t="s">
         <v>191</v>
@@ -5448,13 +5450,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B96" t="s">
         <v>191</v>
-      </c>
-      <c r="C96" t="s">
-        <v>196</v>
       </c>
       <c r="D96" t="s">
         <v>113</v>
@@ -5486,10 +5485,13 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s">
         <v>191</v>
+      </c>
+      <c r="C97" t="s">
+        <v>196</v>
       </c>
       <c r="D97" t="s">
         <v>113</v>
@@ -5513,18 +5515,18 @@
         <v>418</v>
       </c>
       <c r="L97" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="M97" s="5" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B98" t="s">
-        <v>192</v>
-      </c>
-      <c r="C98" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D98" t="s">
         <v>113</v>
@@ -5553,42 +5555,42 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C99" t="s">
-        <v>193</v>
+        <v>196</v>
+      </c>
+      <c r="D99" t="s">
+        <v>113</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G99" s="3">
         <v>1</v>
       </c>
       <c r="H99" s="3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I99" s="3">
         <v>0.9</v>
       </c>
       <c r="J99" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="M99" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B100" t="s">
         <v>191</v>
@@ -5623,13 +5625,13 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B101" t="s">
         <v>191</v>
       </c>
       <c r="C101" t="s">
-        <v>219</v>
+        <v>193</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>212</v>
@@ -5652,16 +5654,19 @@
       <c r="L101" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M101" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B102" t="s">
         <v>191</v>
       </c>
       <c r="C102" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>212</v>
@@ -5687,7 +5692,7 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B103" t="s">
         <v>191</v>
@@ -5716,13 +5721,10 @@
       <c r="L103" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M103" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B104" t="s">
         <v>191</v>
@@ -5757,7 +5759,7 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B105" t="s">
         <v>191</v>
@@ -5792,7 +5794,7 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B106" t="s">
         <v>191</v>
@@ -5821,10 +5823,13 @@
       <c r="L106" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M106" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B107" t="s">
         <v>191</v>
@@ -5853,13 +5858,10 @@
       <c r="L107" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M107" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
         <v>191</v>
@@ -5888,10 +5890,13 @@
       <c r="L108" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M108" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B109" t="s">
         <v>191</v>
@@ -5920,13 +5925,10 @@
       <c r="L109" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M109" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B110" t="s">
         <v>191</v>
@@ -5955,10 +5957,13 @@
       <c r="L110" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M110" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B111" t="s">
         <v>191</v>
@@ -5987,13 +5992,10 @@
       <c r="L111" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M111" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B112" t="s">
         <v>191</v>
@@ -6022,10 +6024,13 @@
       <c r="L112" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M112" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B113" t="s">
         <v>191</v>
@@ -6057,7 +6062,7 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B114" t="s">
         <v>191</v>
@@ -6089,7 +6094,7 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B115" t="s">
         <v>191</v>
@@ -6118,13 +6123,10 @@
       <c r="L115" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M115" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B116" t="s">
         <v>191</v>
@@ -6153,10 +6155,13 @@
       <c r="L116" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M116" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B117" t="s">
         <v>191</v>
@@ -6188,7 +6193,7 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B118" t="s">
         <v>191</v>
@@ -6217,13 +6222,10 @@
       <c r="L118" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M118" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
         <v>191</v>
@@ -6252,10 +6254,13 @@
       <c r="L119" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M119" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B120" t="s">
         <v>191</v>
@@ -6287,7 +6292,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>355</v>
+        <v>136</v>
       </c>
       <c r="B121" t="s">
         <v>191</v>
@@ -6319,7 +6324,7 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B122" t="s">
         <v>191</v>
@@ -6346,15 +6351,12 @@
         <v>421</v>
       </c>
       <c r="L122" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="M122" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>137</v>
+        <v>356</v>
       </c>
       <c r="B123" t="s">
         <v>191</v>
@@ -6389,7 +6391,7 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B124" t="s">
         <v>191</v>
@@ -6398,7 +6400,7 @@
         <v>193</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>525</v>
+        <v>212</v>
       </c>
       <c r="G124" s="3">
         <v>1</v>
@@ -6424,7 +6426,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B125" t="s">
         <v>191</v>
@@ -6433,7 +6435,7 @@
         <v>193</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>212</v>
+        <v>525</v>
       </c>
       <c r="G125" s="3">
         <v>1</v>
@@ -6459,7 +6461,7 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B126" t="s">
         <v>191</v>
@@ -6494,7 +6496,7 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B127" t="s">
         <v>191</v>
@@ -6518,18 +6520,18 @@
         <v>1</v>
       </c>
       <c r="K127" s="5" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="L127" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M127" s="5" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B128" t="s">
         <v>191</v>
@@ -6556,15 +6558,15 @@
         <v>419</v>
       </c>
       <c r="L128" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M128" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B129" t="s">
         <v>191</v>
@@ -6599,7 +6601,7 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B130" t="s">
         <v>191</v>
@@ -6626,12 +6628,15 @@
         <v>419</v>
       </c>
       <c r="L130" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="M130" s="5" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B131" t="s">
         <v>191</v>
@@ -6639,9 +6644,6 @@
       <c r="C131" t="s">
         <v>193</v>
       </c>
-      <c r="D131" t="s">
-        <v>155</v>
-      </c>
       <c r="E131" s="1" t="s">
         <v>212</v>
       </c>
@@ -6666,7 +6668,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B132" t="s">
         <v>191</v>
@@ -6674,6 +6676,9 @@
       <c r="C132" t="s">
         <v>193</v>
       </c>
+      <c r="D132" t="s">
+        <v>155</v>
+      </c>
       <c r="E132" s="1" t="s">
         <v>212</v>
       </c>
@@ -6695,13 +6700,10 @@
       <c r="L132" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M132" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B133" t="s">
         <v>191</v>
@@ -6709,9 +6711,6 @@
       <c r="C133" t="s">
         <v>193</v>
       </c>
-      <c r="D133" t="s">
-        <v>155</v>
-      </c>
       <c r="E133" s="1" t="s">
         <v>212</v>
       </c>
@@ -6739,7 +6738,7 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B134" t="s">
         <v>191</v>
@@ -6747,6 +6746,9 @@
       <c r="C134" t="s">
         <v>193</v>
       </c>
+      <c r="D134" t="s">
+        <v>155</v>
+      </c>
       <c r="E134" s="1" t="s">
         <v>212</v>
       </c>
@@ -6774,7 +6776,7 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B135" t="s">
         <v>191</v>
@@ -6782,9 +6784,6 @@
       <c r="C135" t="s">
         <v>193</v>
       </c>
-      <c r="D135" t="s">
-        <v>155</v>
-      </c>
       <c r="E135" s="1" t="s">
         <v>212</v>
       </c>
@@ -6812,19 +6811,19 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B136" t="s">
         <v>191</v>
       </c>
       <c r="C136" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="D136" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G136" s="3">
         <v>1</v>
@@ -6836,30 +6835,33 @@
         <v>0.9</v>
       </c>
       <c r="J136" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K136" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L136" s="5" t="s">
         <v>427</v>
+      </c>
+      <c r="M136" s="5" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B137" t="s">
         <v>191</v>
       </c>
       <c r="C137" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="D137" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G137" s="3">
         <v>1</v>
@@ -6871,10 +6873,10 @@
         <v>0.9</v>
       </c>
       <c r="J137" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K137" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L137" s="5" t="s">
         <v>427</v>
@@ -6882,7 +6884,7 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B138" t="s">
         <v>191</v>
@@ -6917,7 +6919,7 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B139" t="s">
         <v>191</v>
@@ -6952,28 +6954,34 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>291</v>
+        <v>153</v>
       </c>
       <c r="B140" t="s">
         <v>191</v>
       </c>
+      <c r="C140" t="s">
+        <v>194</v>
+      </c>
+      <c r="D140" t="s">
+        <v>154</v>
+      </c>
       <c r="E140" s="1" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
       <c r="G140" s="3">
         <v>1</v>
       </c>
       <c r="H140" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I140" s="3">
         <v>0.9</v>
       </c>
       <c r="J140" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K140" s="5" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="L140" s="5" t="s">
         <v>427</v>
@@ -6981,7 +6989,7 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B141" t="s">
         <v>191</v>
@@ -7010,7 +7018,7 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B142" t="s">
         <v>191</v>
@@ -7031,7 +7039,7 @@
         <v>0</v>
       </c>
       <c r="K142" s="5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="L142" s="5" t="s">
         <v>427</v>
@@ -7039,13 +7047,10 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B143" t="s">
         <v>191</v>
-      </c>
-      <c r="C143" t="s">
-        <v>196</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>20</v>
@@ -7063,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="K143" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L143" s="5" t="s">
         <v>427</v>
@@ -7071,7 +7076,7 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B144" t="s">
         <v>191</v>
@@ -7095,7 +7100,7 @@
         <v>0</v>
       </c>
       <c r="K144" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L144" s="5" t="s">
         <v>427</v>
@@ -7103,10 +7108,13 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B145" t="s">
         <v>191</v>
+      </c>
+      <c r="C145" t="s">
+        <v>196</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>20</v>
@@ -7124,7 +7132,7 @@
         <v>0</v>
       </c>
       <c r="K145" s="5" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L145" s="5" t="s">
         <v>427</v>
@@ -7132,7 +7140,7 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B146" t="s">
         <v>191</v>
@@ -7153,7 +7161,7 @@
         <v>0</v>
       </c>
       <c r="K146" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="L146" s="5" t="s">
         <v>427</v>
@@ -7161,13 +7169,10 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B147" t="s">
         <v>191</v>
-      </c>
-      <c r="C147" t="s">
-        <v>196</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>20</v>
@@ -7193,10 +7198,13 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B148" t="s">
         <v>191</v>
+      </c>
+      <c r="C148" t="s">
+        <v>196</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>20</v>
@@ -7214,7 +7222,7 @@
         <v>0</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="L148" s="5" t="s">
         <v>427</v>
@@ -7222,7 +7230,7 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B149" t="s">
         <v>191</v>
@@ -7251,7 +7259,7 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B150" t="s">
         <v>191</v>
@@ -7280,7 +7288,7 @@
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B151" t="s">
         <v>191</v>
@@ -7309,7 +7317,7 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B152" t="s">
         <v>191</v>
@@ -7338,7 +7346,7 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B153" t="s">
         <v>191</v>
@@ -7367,7 +7375,7 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B154" t="s">
         <v>191</v>
@@ -7396,7 +7404,7 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B155" t="s">
         <v>191</v>
@@ -7425,7 +7433,7 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B156" t="s">
         <v>191</v>
@@ -7454,7 +7462,7 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B157" t="s">
         <v>191</v>
@@ -7483,7 +7491,7 @@
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B158" t="s">
         <v>191</v>
@@ -7512,7 +7520,7 @@
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="B159" t="s">
         <v>191</v>
@@ -7541,7 +7549,7 @@
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="B160" t="s">
         <v>191</v>
@@ -7570,7 +7578,7 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B161" t="s">
         <v>191</v>
@@ -7599,13 +7607,10 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B162" t="s">
         <v>191</v>
-      </c>
-      <c r="D162" t="s">
-        <v>87</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>20</v>
@@ -7631,13 +7636,13 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B163" t="s">
         <v>191</v>
       </c>
-      <c r="C163" t="s">
-        <v>196</v>
+      <c r="D163" t="s">
+        <v>87</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>20</v>
@@ -7655,7 +7660,7 @@
         <v>0</v>
       </c>
       <c r="K163" s="5" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="L163" s="5" t="s">
         <v>427</v>
@@ -7663,10 +7668,13 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B164" t="s">
         <v>191</v>
+      </c>
+      <c r="C164" t="s">
+        <v>196</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>20</v>
@@ -7684,24 +7692,18 @@
         <v>0</v>
       </c>
       <c r="K164" s="5" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="L164" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="M164" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B165" t="s">
         <v>191</v>
-      </c>
-      <c r="C165" t="s">
-        <v>198</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>20</v>
@@ -7719,7 +7721,7 @@
         <v>0</v>
       </c>
       <c r="K165" s="5" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="L165" s="5" t="s">
         <v>427</v>
@@ -7730,10 +7732,13 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="B166" t="s">
         <v>191</v>
+      </c>
+      <c r="C166" t="s">
+        <v>198</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>20</v>
@@ -7751,7 +7756,7 @@
         <v>0</v>
       </c>
       <c r="K166" s="5" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="L166" s="5" t="s">
         <v>427</v>
@@ -7762,7 +7767,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="B167" t="s">
         <v>191</v>
@@ -7794,7 +7799,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B168" t="s">
         <v>191</v>
@@ -7826,7 +7831,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B169" t="s">
         <v>191</v>
@@ -7852,10 +7857,13 @@
       <c r="L169" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M169" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B170" t="s">
         <v>191</v>
@@ -7884,13 +7892,10 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B171" t="s">
         <v>191</v>
-      </c>
-      <c r="C171" t="s">
-        <v>196</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>20</v>
@@ -7908,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="K171" s="5" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="L171" s="5" t="s">
         <v>427</v>
@@ -7916,10 +7921,13 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B172" t="s">
         <v>191</v>
+      </c>
+      <c r="C172" t="s">
+        <v>196</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>20</v>
@@ -7937,7 +7945,7 @@
         <v>0</v>
       </c>
       <c r="K172" s="5" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="L172" s="5" t="s">
         <v>427</v>
@@ -7945,7 +7953,7 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B173" t="s">
         <v>191</v>
@@ -7974,7 +7982,7 @@
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B174" t="s">
         <v>191</v>
@@ -8003,7 +8011,7 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B175" t="s">
         <v>191</v>
@@ -8032,7 +8040,7 @@
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B176" t="s">
         <v>191</v>
@@ -8061,13 +8069,10 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B177" t="s">
         <v>191</v>
-      </c>
-      <c r="C177" t="s">
-        <v>198</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>20</v>
@@ -8085,21 +8090,21 @@
         <v>0</v>
       </c>
       <c r="K177" s="5" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="L177" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="M177" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B178" t="s">
         <v>191</v>
+      </c>
+      <c r="C178" t="s">
+        <v>198</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>20</v>
@@ -8117,7 +8122,7 @@
         <v>0</v>
       </c>
       <c r="K178" s="5" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="L178" s="5" t="s">
         <v>427</v>
@@ -8128,7 +8133,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B179" t="s">
         <v>191</v>
@@ -8160,7 +8165,7 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B180" t="s">
         <v>191</v>
@@ -8181,18 +8186,18 @@
         <v>0</v>
       </c>
       <c r="K180" s="5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L180" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M180" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B181" t="s">
         <v>191</v>
@@ -8224,13 +8229,10 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B182" t="s">
         <v>191</v>
-      </c>
-      <c r="C182" t="s">
-        <v>196</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>20</v>
@@ -8259,10 +8261,13 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B183" t="s">
         <v>191</v>
+      </c>
+      <c r="C183" t="s">
+        <v>196</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>20</v>
@@ -8283,18 +8288,18 @@
         <v>418</v>
       </c>
       <c r="L183" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="M183" s="5" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B184" t="s">
         <v>191</v>
-      </c>
-      <c r="C184" t="s">
-        <v>196</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>20</v>
@@ -8320,42 +8325,39 @@
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B185" t="s">
         <v>191</v>
       </c>
       <c r="C185" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>212</v>
+        <v>20</v>
       </c>
       <c r="G185" s="3">
         <v>1</v>
       </c>
       <c r="H185" s="3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I185" s="3">
         <v>0.9</v>
       </c>
       <c r="J185" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K185" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="L185" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="M185" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B186" t="s">
         <v>191</v>
@@ -8390,7 +8392,7 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B187" t="s">
         <v>191</v>
@@ -8419,10 +8421,13 @@
       <c r="L187" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M187" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B188" t="s">
         <v>191</v>
@@ -8454,7 +8459,7 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B189" t="s">
         <v>191</v>
@@ -8483,13 +8488,10 @@
       <c r="L189" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M189" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B190" t="s">
         <v>191</v>
@@ -8524,7 +8526,7 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="B191" t="s">
         <v>191</v>
@@ -8559,7 +8561,7 @@
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B192" t="s">
         <v>191</v>
@@ -8588,10 +8590,13 @@
       <c r="L192" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M192" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B193" t="s">
         <v>191</v>
@@ -8620,13 +8625,10 @@
       <c r="L193" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M193" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B194" t="s">
         <v>191</v>
@@ -8655,10 +8657,13 @@
       <c r="L194" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M194" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
       <c r="B195" t="s">
         <v>191</v>
@@ -8687,13 +8692,10 @@
       <c r="L195" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M195" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B196" t="s">
         <v>191</v>
@@ -8722,10 +8724,13 @@
       <c r="L196" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M196" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B197" t="s">
         <v>191</v>
@@ -8754,13 +8759,10 @@
       <c r="L197" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M197" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B198" t="s">
         <v>191</v>
@@ -8789,10 +8791,13 @@
       <c r="L198" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M198" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B199" t="s">
         <v>191</v>
@@ -8824,7 +8829,7 @@
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B200" t="s">
         <v>191</v>
@@ -8856,7 +8861,7 @@
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B201" t="s">
         <v>191</v>
@@ -8885,13 +8890,10 @@
       <c r="L201" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M201" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B202" t="s">
         <v>191</v>
@@ -8920,10 +8922,13 @@
       <c r="L202" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M202" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B203" t="s">
         <v>191</v>
@@ -8955,7 +8960,7 @@
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B204" t="s">
         <v>191</v>
@@ -8984,13 +8989,10 @@
       <c r="L204" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M204" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B205" t="s">
         <v>191</v>
@@ -9019,10 +9021,13 @@
       <c r="L205" s="5" t="s">
         <v>427</v>
       </c>
+      <c r="M205" s="5" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B206" t="s">
         <v>191</v>
@@ -9054,7 +9059,7 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B207" t="s">
         <v>191</v>
@@ -9086,7 +9091,7 @@
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B208" t="s">
         <v>191</v>
@@ -9113,15 +9118,12 @@
         <v>421</v>
       </c>
       <c r="L208" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="M208" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B209" t="s">
         <v>191</v>
@@ -9156,7 +9158,7 @@
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B210" t="s">
         <v>191</v>
@@ -9191,7 +9193,7 @@
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B211" t="s">
         <v>191</v>
@@ -9226,7 +9228,7 @@
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B212" t="s">
         <v>191</v>
@@ -9261,7 +9263,7 @@
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B213" t="s">
         <v>191</v>
@@ -9285,18 +9287,18 @@
         <v>1</v>
       </c>
       <c r="K213" s="5" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="L213" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M213" s="5" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B214" t="s">
         <v>191</v>
@@ -9323,15 +9325,15 @@
         <v>419</v>
       </c>
       <c r="L214" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="M214" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B215" t="s">
         <v>191</v>
@@ -9366,7 +9368,7 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B216" t="s">
         <v>191</v>
@@ -9393,12 +9395,15 @@
         <v>419</v>
       </c>
       <c r="L216" s="5" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="M216" s="5" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B217" t="s">
         <v>191</v>
@@ -9430,7 +9435,7 @@
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B218" t="s">
         <v>191</v>
@@ -9459,13 +9464,10 @@
       <c r="L218" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="M218" s="5" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B219" t="s">
         <v>191</v>
@@ -9500,7 +9502,7 @@
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B220" t="s">
         <v>191</v>
@@ -9535,7 +9537,7 @@
     </row>
     <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B221" t="s">
         <v>191</v>
@@ -9570,16 +9572,16 @@
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B222" t="s">
         <v>191</v>
       </c>
       <c r="C222" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G222" s="3">
         <v>1</v>
@@ -9591,27 +9593,30 @@
         <v>0.9</v>
       </c>
       <c r="J222" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K222" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L222" s="5" t="s">
         <v>427</v>
+      </c>
+      <c r="M222" s="5" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B223" t="s">
         <v>191</v>
       </c>
       <c r="C223" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G223" s="3">
         <v>1</v>
@@ -9623,10 +9628,10 @@
         <v>0.9</v>
       </c>
       <c r="J223" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K223" s="5" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L223" s="5" t="s">
         <v>427</v>
@@ -9634,7 +9639,7 @@
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B224" t="s">
         <v>191</v>
@@ -9666,7 +9671,7 @@
     </row>
     <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B225" t="s">
         <v>191</v>
@@ -9698,42 +9703,39 @@
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>168</v>
+        <v>379</v>
       </c>
       <c r="B226" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C226" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G226" s="3">
         <v>1</v>
       </c>
       <c r="H226" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I226" s="3">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="J226" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K226" s="5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="L226" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="M226" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B227" t="s">
         <v>186</v>
@@ -9768,7 +9770,7 @@
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B228" t="s">
         <v>186</v>
@@ -9803,7 +9805,7 @@
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B229" t="s">
         <v>186</v>
@@ -9838,7 +9840,7 @@
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B230" t="s">
         <v>186</v>
@@ -9873,7 +9875,7 @@
     </row>
     <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B231" t="s">
         <v>186</v>
@@ -9908,7 +9910,7 @@
     </row>
     <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B232" t="s">
         <v>186</v>
@@ -9943,7 +9945,7 @@
     </row>
     <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>289</v>
+        <v>176</v>
       </c>
       <c r="B233" t="s">
         <v>186</v>
@@ -9978,10 +9980,10 @@
     </row>
     <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>167</v>
+        <v>289</v>
       </c>
       <c r="B234" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="C234" t="s">
         <v>222</v>
@@ -10013,10 +10015,10 @@
     </row>
     <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B235" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="C235" t="s">
         <v>222</v>
@@ -10048,7 +10050,7 @@
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B236" t="s">
         <v>186</v>
@@ -10083,10 +10085,10 @@
     </row>
     <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B237" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C237" t="s">
         <v>222</v>
@@ -10118,10 +10120,10 @@
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B238" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="C238" t="s">
         <v>222</v>
@@ -10153,7 +10155,7 @@
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B239" t="s">
         <v>186</v>
@@ -10188,7 +10190,7 @@
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B240" t="s">
         <v>186</v>
@@ -10223,7 +10225,7 @@
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="B241" t="s">
         <v>186</v>
@@ -10258,7 +10260,7 @@
     </row>
     <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B242" t="s">
         <v>186</v>
@@ -10288,12 +10290,12 @@
         <v>428</v>
       </c>
       <c r="M242" s="5" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B243" t="s">
         <v>186</v>
@@ -10323,15 +10325,15 @@
         <v>428</v>
       </c>
       <c r="M243" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B244" t="s">
-        <v>19</v>
+        <v>186</v>
       </c>
       <c r="C244" t="s">
         <v>222</v>
@@ -10357,14 +10359,16 @@
       <c r="L244" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M244" s="6"/>
+      <c r="M244" s="5" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="B245" t="s">
-        <v>186</v>
+        <v>19</v>
       </c>
       <c r="C245" t="s">
         <v>222</v>
@@ -10390,13 +10394,11 @@
       <c r="L245" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M245" s="5" t="s">
-        <v>431</v>
-      </c>
+      <c r="M245" s="6"/>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B246" t="s">
         <v>186</v>
@@ -10431,19 +10433,19 @@
     </row>
     <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="B247" t="s">
         <v>186</v>
       </c>
       <c r="C247" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E247" s="1" t="s">
         <v>214</v>
       </c>
       <c r="G247" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H247" s="3">
         <v>0.8</v>
@@ -10466,7 +10468,7 @@
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="B248" t="s">
         <v>186</v>
@@ -10501,7 +10503,7 @@
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B249" t="s">
         <v>186</v>
@@ -10536,7 +10538,7 @@
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B250" t="s">
         <v>186</v>
@@ -10566,12 +10568,12 @@
         <v>428</v>
       </c>
       <c r="M250" s="5" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B251" t="s">
         <v>186</v>
@@ -10601,12 +10603,12 @@
         <v>428</v>
       </c>
       <c r="M251" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B252" t="s">
         <v>186</v>
@@ -10635,11 +10637,13 @@
       <c r="L252" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M252" s="6"/>
+      <c r="M252" s="5" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B253" t="s">
         <v>186</v>
@@ -10668,25 +10672,23 @@
       <c r="L253" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M253" s="5" t="s">
-        <v>431</v>
-      </c>
+      <c r="M253" s="6"/>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B254" t="s">
         <v>186</v>
       </c>
       <c r="C254" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="E254" s="1" t="s">
         <v>214</v>
       </c>
       <c r="G254" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H254" s="3">
         <v>0.8</v>
@@ -10709,7 +10711,7 @@
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B255" t="s">
         <v>186</v>
@@ -10744,16 +10746,16 @@
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>271</v>
+        <v>185</v>
       </c>
       <c r="B256" t="s">
-        <v>19</v>
+        <v>186</v>
       </c>
       <c r="C256" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="G256" s="3">
         <v>1</v>
@@ -10779,7 +10781,7 @@
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B257" t="s">
         <v>19</v>
@@ -10814,7 +10816,7 @@
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B258" t="s">
         <v>19</v>
@@ -10849,7 +10851,7 @@
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B259" t="s">
         <v>19</v>
@@ -10884,7 +10886,7 @@
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B260" t="s">
         <v>19</v>
@@ -10919,7 +10921,7 @@
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B261" t="s">
         <v>19</v>
@@ -10954,7 +10956,7 @@
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B262" t="s">
         <v>19</v>
@@ -10989,7 +10991,7 @@
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B263" t="s">
         <v>19</v>
@@ -11024,7 +11026,7 @@
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B264" t="s">
         <v>19</v>
@@ -11059,7 +11061,7 @@
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B265" t="s">
         <v>19</v>
@@ -11094,7 +11096,7 @@
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B266" t="s">
         <v>19</v>
@@ -11129,7 +11131,7 @@
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B267" t="s">
         <v>19</v>
@@ -11164,7 +11166,7 @@
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B268" t="s">
         <v>19</v>
@@ -11199,7 +11201,7 @@
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B269" t="s">
         <v>19</v>
@@ -11234,7 +11236,7 @@
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B270" t="s">
         <v>19</v>
@@ -11269,7 +11271,7 @@
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="B271" t="s">
         <v>19</v>
@@ -11304,7 +11306,7 @@
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B272" t="s">
         <v>19</v>
@@ -11334,12 +11336,12 @@
         <v>428</v>
       </c>
       <c r="M272" s="5" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="273" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B273" t="s">
         <v>19</v>
@@ -11369,12 +11371,12 @@
         <v>428</v>
       </c>
       <c r="M273" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B274" t="s">
         <v>19</v>
@@ -11403,11 +11405,13 @@
       <c r="L274" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M274" s="6"/>
+      <c r="M274" s="5" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="B275" t="s">
         <v>19</v>
@@ -11436,13 +11440,11 @@
       <c r="L275" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M275" s="5" t="s">
-        <v>431</v>
-      </c>
+      <c r="M275" s="6"/>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B276" t="s">
         <v>19</v>
@@ -11477,19 +11479,19 @@
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="B277" t="s">
         <v>19</v>
       </c>
       <c r="C277" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E277" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G277" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H277" s="3">
         <v>0.8</v>
@@ -11512,7 +11514,7 @@
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="B278" t="s">
         <v>19</v>
@@ -11547,7 +11549,7 @@
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="B279" t="s">
         <v>19</v>
@@ -11582,7 +11584,7 @@
     </row>
     <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B280" t="s">
         <v>19</v>
@@ -11612,12 +11614,12 @@
         <v>428</v>
       </c>
       <c r="M280" s="5" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B281" t="s">
         <v>19</v>
@@ -11647,12 +11649,12 @@
         <v>428</v>
       </c>
       <c r="M281" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B282" t="s">
         <v>19</v>
@@ -11681,11 +11683,13 @@
       <c r="L282" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M282" s="6"/>
+      <c r="M282" s="5" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="B283" t="s">
         <v>19</v>
@@ -11714,25 +11718,23 @@
       <c r="L283" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="M283" s="5" t="s">
-        <v>431</v>
-      </c>
+      <c r="M283" s="6"/>
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B284" t="s">
         <v>19</v>
       </c>
       <c r="C284" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="E284" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G284" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H284" s="3">
         <v>0.8</v>
@@ -11755,7 +11757,7 @@
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B285" t="s">
         <v>19</v>
@@ -11785,6 +11787,41 @@
         <v>428</v>
       </c>
       <c r="M285" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>288</v>
+      </c>
+      <c r="B286" t="s">
+        <v>19</v>
+      </c>
+      <c r="C286" t="s">
+        <v>187</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G286" s="3">
+        <v>1</v>
+      </c>
+      <c r="H286" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="I286" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="J286" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K286" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="L286" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="M286" s="5" t="s">
         <v>431</v>
       </c>
     </row>
@@ -12042,7 +12079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>